<commit_message>
dataloader modified and environment data only train/infer supported
</commit_message>
<xml_diff>
--- a/dataset/2nd_data/beak/beak_env_detail_data.xlsx
+++ b/dataset/2nd_data/beak/beak_env_detail_data.xlsx
@@ -384,332 +384,332 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>dew point (Td)</t>
+          <t>이슬점(Td)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>HD</t>
+          <t>증산(HD)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>atmospheric pressure</t>
+          <t>대기압</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>pws</t>
+          <t>PWS(?)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>W (moisture content)</t>
+          <t>수분량</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>h (enthalpy)</t>
+          <t>엔탈피</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>v (specific volume)</t>
+          <t>비부피</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>rho (density)</t>
+          <t>밀도</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>pw (Partial pressure) water vapor</t>
+          <t>PW(?)수증기</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Absolute Humidity (AH)</t>
+          <t>절대습도</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>absoluteAH</t>
+          <t>절대AH(?)</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>실내온도_std</t>
+          <t>실내온도표준편차</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>실내습도_std</t>
+          <t>실내습도표준편차</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>dew point (Td)_std</t>
+          <t>이슬점(Td)표준편차</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>HD_std</t>
+          <t>증산(HD)표준편차</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>atmospheric pressure_std</t>
+          <t>대기압표준편차</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>pws_std</t>
+          <t>PWS(?)표준편차</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>W (moisture content)_std</t>
+          <t>수분량표준편차</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>h (enthalpy)_std</t>
+          <t>엔탈피표준편차</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>v (specific volume)_std</t>
+          <t>비부피표준편차</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>rho (density)_std</t>
+          <t>밀도표준편차</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>pw (Partial pressure) water vapor_std</t>
+          <t>PW(?)수증기표준편차</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>Absolute Humidity (AH)_std</t>
+          <t>절대습도표준편차</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>absoluteAH_std</t>
+          <t>절대AH(?)표준편차</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>실내온도_min</t>
+          <t>최소실내온도</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>실내습도_min</t>
+          <t>최소실내습도</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>dew point (Td)_min</t>
+          <t>최소이슬점(Td)</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>HD_min</t>
+          <t>최소증산(HD)</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>atmospheric pressure_min</t>
+          <t>최소대기압</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>pws_min</t>
+          <t>최소PWS(?)</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>W (moisture content)_min</t>
+          <t>최소수분량</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>h (enthalpy)_min</t>
+          <t>최소엔탈피</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>v (specific volume)_min</t>
+          <t>최소비부피</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>rho (density)_min</t>
+          <t>최소밀도</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>pw (Partial pressure) water vapor_min</t>
+          <t>최소PW(?)수증기</t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t>Absolute Humidity (AH)_min</t>
+          <t>최소절대습도</t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
-          <t>absoluteAH_min</t>
+          <t>최소절대AH(?)</t>
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
         <is>
-          <t>실내온도_max</t>
+          <t>최대실내온도</t>
         </is>
       </c>
       <c r="AP1" s="1" t="inlineStr">
         <is>
-          <t>실내습도_max</t>
+          <t>최대실내습도</t>
         </is>
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
-          <t>dew point (Td)_max</t>
+          <t>최대이슬점(Td)</t>
         </is>
       </c>
       <c r="AR1" s="1" t="inlineStr">
         <is>
-          <t>HD_max</t>
+          <t>최대증산(HD)</t>
         </is>
       </c>
       <c r="AS1" s="1" t="inlineStr">
         <is>
-          <t>atmospheric pressure_max</t>
+          <t>최대대기압</t>
         </is>
       </c>
       <c r="AT1" s="1" t="inlineStr">
         <is>
-          <t>pws_max</t>
+          <t>최대PWS(?)</t>
         </is>
       </c>
       <c r="AU1" s="1" t="inlineStr">
         <is>
-          <t>W (moisture content)_max</t>
+          <t>최대수분량</t>
         </is>
       </c>
       <c r="AV1" s="1" t="inlineStr">
         <is>
-          <t>h (enthalpy)_max</t>
+          <t>최대엔탈피</t>
         </is>
       </c>
       <c r="AW1" s="1" t="inlineStr">
         <is>
-          <t>v (specific volume)_max</t>
+          <t>최대비부피</t>
         </is>
       </c>
       <c r="AX1" s="1" t="inlineStr">
         <is>
-          <t>rho (density)_max</t>
+          <t>최대밀도</t>
         </is>
       </c>
       <c r="AY1" s="1" t="inlineStr">
         <is>
-          <t>pw (Partial pressure) water vapor_max</t>
+          <t>최대PW(?)수증기</t>
         </is>
       </c>
       <c r="AZ1" s="1" t="inlineStr">
         <is>
-          <t>Absolute Humidity (AH)_max</t>
+          <t>최대절대습도</t>
         </is>
       </c>
       <c r="BA1" s="1" t="inlineStr">
         <is>
-          <t>absoluteAH_max</t>
+          <t>최대절대AH(?)</t>
         </is>
       </c>
       <c r="BB1" s="1" t="inlineStr">
         <is>
-          <t>am_suitable_HD</t>
+          <t>오전적정증산(HD)누적시간</t>
         </is>
       </c>
       <c r="BC1" s="1" t="inlineStr">
         <is>
-          <t>sun_suitable_HD</t>
+          <t>일출일몰적정증산(HD)누적시간</t>
         </is>
       </c>
       <c r="BD1" s="1" t="inlineStr">
         <is>
-          <t>day_suitable_HD</t>
+          <t>하루적정증산(HD)누적시간</t>
         </is>
       </c>
       <c r="BE1" s="1" t="inlineStr">
         <is>
-          <t>pm_unsuitable_HD</t>
+          <t>오후심각증산(HD)누적시간</t>
         </is>
       </c>
       <c r="BF1" s="1" t="inlineStr">
         <is>
-          <t>am_unsuitable_HD</t>
+          <t>오전심각증산(HD)누적시간</t>
         </is>
       </c>
       <c r="BG1" s="1" t="inlineStr">
         <is>
-          <t>low_temperature</t>
+          <t>12도이하온도누적시간</t>
         </is>
       </c>
       <c r="BH1" s="1" t="inlineStr">
         <is>
-          <t>high_temperature</t>
+          <t>30도이상온도누적시간</t>
         </is>
       </c>
       <c r="BI1" s="1" t="inlineStr">
         <is>
-          <t>suitable_temperature</t>
+          <t>적정온도누적시간</t>
         </is>
       </c>
       <c r="BJ1" s="1" t="inlineStr">
         <is>
-          <t>daytime_temperature</t>
+          <t>주간평균온도</t>
         </is>
       </c>
       <c r="BK1" s="1" t="inlineStr">
         <is>
-          <t>nighttime_temperature</t>
+          <t>야간평균온도</t>
         </is>
       </c>
       <c r="BL1" s="1" t="inlineStr">
         <is>
-          <t>afternoon_temperature</t>
+          <t>오후부터일몰까지평균온도</t>
         </is>
       </c>
       <c r="BM1" s="1" t="inlineStr">
         <is>
-          <t>suitable_humidity_time</t>
+          <t>적정습도누적시간</t>
         </is>
       </c>
       <c r="BN1" s="1" t="inlineStr">
         <is>
-          <t>sunrise_diff</t>
+          <t>일출전후한시간평균온도</t>
         </is>
       </c>
       <c r="BO1" s="1" t="inlineStr">
         <is>
-          <t>sunset_diff</t>
+          <t>일몰전후한시간평균온도</t>
         </is>
       </c>
       <c r="BP1" s="1" t="inlineStr">
         <is>
-          <t>suitable_temperature_diff_lowerbound</t>
+          <t>적정온도변화폭(하위)</t>
         </is>
       </c>
       <c r="BQ1" s="1" t="inlineStr">
         <is>
-          <t>suitable_temperature_diff_upperbound</t>
+          <t>적정온도변화폭(상위)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
demanded environment features added
</commit_message>
<xml_diff>
--- a/dataset/2nd_data/beak/beak_env_detail_data.xlsx
+++ b/dataset/2nd_data/beak/beak_env_detail_data.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BQ85"/>
+  <dimension ref="A1:BS84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -679,37 +679,47 @@
       </c>
       <c r="BK1" s="1" t="inlineStr">
         <is>
-          <t>야간평균온도</t>
-        </is>
-      </c>
-      <c r="BL1" s="1" t="inlineStr">
-        <is>
           <t>오후부터일몰까지평균온도</t>
         </is>
       </c>
-      <c r="BM1" s="1" t="inlineStr">
+      <c r="BL1" s="1" t="inlineStr">
         <is>
           <t>적정습도누적시간</t>
         </is>
       </c>
-      <c r="BN1" s="1" t="inlineStr">
+      <c r="BM1" s="1" t="inlineStr">
         <is>
           <t>일출전후한시간평균온도</t>
         </is>
       </c>
-      <c r="BO1" s="1" t="inlineStr">
+      <c r="BN1" s="1" t="inlineStr">
         <is>
           <t>일몰전후한시간평균온도</t>
         </is>
       </c>
-      <c r="BP1" s="1" t="inlineStr">
+      <c r="BO1" s="1" t="inlineStr">
         <is>
           <t>적정온도변화폭(하위)</t>
         </is>
       </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>적정온도변화폭(상위)</t>
+        </is>
+      </c>
       <c r="BQ1" s="1" t="inlineStr">
         <is>
-          <t>적정온도변화폭(상위)</t>
+          <t>야간평균온도</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>일몰일출적합증산(HD)누적시간</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>주야간온도차이</t>
         </is>
       </c>
     </row>
@@ -901,25 +911,31 @@
         <v>21.73271446863007</v>
       </c>
       <c r="BK2" t="n">
-        <v>17.54691489361711</v>
+        <v>24.11836104513072</v>
       </c>
       <c r="BL2" t="n">
-        <v>24.11836104513072</v>
+        <v>0.8166666666666667</v>
       </c>
       <c r="BM2" t="n">
-        <v>0.8166666666666667</v>
+        <v>0.2899999999999991</v>
       </c>
       <c r="BN2" t="n">
-        <v>0.2899999999999991</v>
+        <v>2.310000000000002</v>
       </c>
       <c r="BO2" t="n">
-        <v>2.310000000000002</v>
+        <v>-0.8100000000000005</v>
       </c>
       <c r="BP2" t="n">
-        <v>-0.8100000000000005</v>
+        <v>3.5</v>
       </c>
       <c r="BQ2" t="n">
-        <v>3.5</v>
+        <v>17.51379362670719</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>7.916666666666667</v>
+      </c>
+      <c r="BS2" t="n">
+        <v>4.218920841922877</v>
       </c>
     </row>
     <row r="3">
@@ -1110,25 +1126,31 @@
         <v>17.43607692307704</v>
       </c>
       <c r="BK3" t="n">
-        <v>15.71306525037935</v>
+        <v>19.78714964370552</v>
       </c>
       <c r="BL3" t="n">
-        <v>19.78714964370552</v>
+        <v>5.683333333333334</v>
       </c>
       <c r="BM3" t="n">
-        <v>5.683333333333334</v>
+        <v>1.41</v>
       </c>
       <c r="BN3" t="n">
-        <v>1.41</v>
+        <v>2.199999999999999</v>
       </c>
       <c r="BO3" t="n">
-        <v>2.199999999999999</v>
+        <v>-2.609999999999999</v>
       </c>
       <c r="BP3" t="n">
-        <v>-2.609999999999999</v>
+        <v>-2.710000000000001</v>
       </c>
       <c r="BQ3" t="n">
-        <v>-2.710000000000001</v>
+        <v>14.17154779969653</v>
+      </c>
+      <c r="BR3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS3" t="n">
+        <v>3.264529123380502</v>
       </c>
     </row>
     <row r="4">
@@ -1319,25 +1341,31 @@
         <v>19.37821428571441</v>
       </c>
       <c r="BK4" t="n">
-        <v>14.29080424886191</v>
+        <v>21.33303703703709</v>
       </c>
       <c r="BL4" t="n">
-        <v>21.33303703703709</v>
+        <v>0</v>
       </c>
       <c r="BM4" t="n">
-        <v>0</v>
+        <v>1.700000000000001</v>
       </c>
       <c r="BN4" t="n">
-        <v>1.700000000000001</v>
+        <v>4.210000000000001</v>
       </c>
       <c r="BO4" t="n">
-        <v>4.210000000000001</v>
+        <v>-2.81</v>
       </c>
       <c r="BP4" t="n">
-        <v>-2.81</v>
+        <v>3.199999999999999</v>
       </c>
       <c r="BQ4" t="n">
-        <v>3.199999999999999</v>
+        <v>14.19098784194526</v>
+      </c>
+      <c r="BR4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS4" t="n">
+        <v>5.18722644376915</v>
       </c>
     </row>
     <row r="5">
@@ -1528,25 +1556,31 @@
         <v>18.76166666666678</v>
       </c>
       <c r="BK5" t="n">
-        <v>14.78430091185413</v>
+        <v>20.27095011876487</v>
       </c>
       <c r="BL5" t="n">
-        <v>20.27095011876487</v>
+        <v>0</v>
       </c>
       <c r="BM5" t="n">
-        <v>0</v>
+        <v>0.3100000000000005</v>
       </c>
       <c r="BN5" t="n">
-        <v>0.3100000000000005</v>
+        <v>1.399999999999999</v>
       </c>
       <c r="BO5" t="n">
-        <v>1.399999999999999</v>
+        <v>-2.81</v>
       </c>
       <c r="BP5" t="n">
-        <v>-2.81</v>
+        <v>0</v>
       </c>
       <c r="BQ5" t="n">
-        <v>0</v>
+        <v>15.23522003034902</v>
+      </c>
+      <c r="BR5" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="BS5" t="n">
+        <v>3.526446636317759</v>
       </c>
     </row>
     <row r="6">
@@ -1737,25 +1771,31 @@
         <v>18.13081606217628</v>
       </c>
       <c r="BK6" t="n">
-        <v>14.58438543247345</v>
+        <v>20.4760332541568</v>
       </c>
       <c r="BL6" t="n">
-        <v>20.4760332541568</v>
+        <v>0</v>
       </c>
       <c r="BM6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN6" t="n">
-        <v>1</v>
+        <v>3.489999999999998</v>
       </c>
       <c r="BO6" t="n">
-        <v>3.489999999999998</v>
+        <v>-2.4</v>
       </c>
       <c r="BP6" t="n">
-        <v>-2.4</v>
+        <v>-2.210000000000001</v>
       </c>
       <c r="BQ6" t="n">
-        <v>-2.210000000000001</v>
+        <v>14.43637329286799</v>
+      </c>
+      <c r="BR6" t="n">
+        <v>3.616666666666667</v>
+      </c>
+      <c r="BS6" t="n">
+        <v>3.694442769308282</v>
       </c>
     </row>
     <row r="7">
@@ -1946,25 +1986,31 @@
         <v>19.32714468629976</v>
       </c>
       <c r="BK7" t="n">
-        <v>14.40474885844752</v>
+        <v>22.12273159144899</v>
       </c>
       <c r="BL7" t="n">
-        <v>22.12273159144899</v>
+        <v>0</v>
       </c>
       <c r="BM7" t="n">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="BN7" t="n">
-        <v>1.4</v>
+        <v>2.699999999999999</v>
       </c>
       <c r="BO7" t="n">
-        <v>2.699999999999999</v>
+        <v>-2.4</v>
       </c>
       <c r="BP7" t="n">
-        <v>-2.4</v>
+        <v>0.1000000000000014</v>
       </c>
       <c r="BQ7" t="n">
-        <v>0.1000000000000014</v>
+        <v>14.48665130568356</v>
+      </c>
+      <c r="BR7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS7" t="n">
+        <v>4.840493380616202</v>
       </c>
     </row>
     <row r="8">
@@ -2155,25 +2201,31 @@
         <v>18.44128040973122</v>
       </c>
       <c r="BK8" t="n">
-        <v>14.57186830015317</v>
+        <v>20.62610451306418</v>
       </c>
       <c r="BL8" t="n">
-        <v>20.62610451306418</v>
+        <v>0</v>
       </c>
       <c r="BM8" t="n">
-        <v>0</v>
+        <v>1.09</v>
       </c>
       <c r="BN8" t="n">
-        <v>1.09</v>
+        <v>2.300000000000001</v>
       </c>
       <c r="BO8" t="n">
-        <v>2.300000000000001</v>
+        <v>-2.4</v>
       </c>
       <c r="BP8" t="n">
-        <v>-2.4</v>
+        <v>-1.399999999999999</v>
       </c>
       <c r="BQ8" t="n">
-        <v>-1.399999999999999</v>
+        <v>14.42584218512891</v>
+      </c>
+      <c r="BR8" t="n">
+        <v>2.466666666666667</v>
+      </c>
+      <c r="BS8" t="n">
+        <v>4.01543822460231</v>
       </c>
     </row>
     <row r="9">
@@ -2364,25 +2416,31 @@
         <v>18.99086340206196</v>
       </c>
       <c r="BK9" t="n">
-        <v>14.6654476479515</v>
+        <v>20.94336538461541</v>
       </c>
       <c r="BL9" t="n">
-        <v>20.94336538461541</v>
+        <v>0</v>
       </c>
       <c r="BM9" t="n">
-        <v>0</v>
+        <v>1.110000000000001</v>
       </c>
       <c r="BN9" t="n">
-        <v>1.110000000000001</v>
+        <v>3.309999999999999</v>
       </c>
       <c r="BO9" t="n">
-        <v>3.309999999999999</v>
+        <v>-2.4</v>
       </c>
       <c r="BP9" t="n">
-        <v>-2.4</v>
+        <v>-0.3999999999999986</v>
       </c>
       <c r="BQ9" t="n">
-        <v>-0.3999999999999986</v>
+        <v>14.77216923076928</v>
+      </c>
+      <c r="BR9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS9" t="n">
+        <v>4.218694171292684</v>
       </c>
     </row>
     <row r="10">
@@ -2573,25 +2631,31 @@
         <v>19.26900516795876</v>
       </c>
       <c r="BK10" t="n">
-        <v>15.01247692307696</v>
+        <v>21.6315347721823</v>
       </c>
       <c r="BL10" t="n">
-        <v>21.6315347721823</v>
+        <v>0</v>
       </c>
       <c r="BM10" t="n">
-        <v>0</v>
+        <v>1.200000000000001</v>
       </c>
       <c r="BN10" t="n">
-        <v>1.200000000000001</v>
+        <v>3</v>
       </c>
       <c r="BO10" t="n">
-        <v>3</v>
+        <v>-2.4</v>
       </c>
       <c r="BP10" t="n">
-        <v>-2.4</v>
+        <v>-1.609999999999999</v>
       </c>
       <c r="BQ10" t="n">
-        <v>-1.609999999999999</v>
+        <v>14.85311248073963</v>
+      </c>
+      <c r="BR10" t="n">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="BS10" t="n">
+        <v>4.415892687219129</v>
       </c>
     </row>
     <row r="11">
@@ -2782,25 +2846,31 @@
         <v>21.13298177083343</v>
       </c>
       <c r="BK11" t="n">
-        <v>15.51870866141739</v>
+        <v>23.37947115384622</v>
       </c>
       <c r="BL11" t="n">
-        <v>23.37947115384622</v>
+        <v>0</v>
       </c>
       <c r="BM11" t="n">
-        <v>0</v>
+        <v>1.110000000000001</v>
       </c>
       <c r="BN11" t="n">
-        <v>1.110000000000001</v>
+        <v>3.710000000000001</v>
       </c>
       <c r="BO11" t="n">
-        <v>3.710000000000001</v>
+        <v>-2.5</v>
       </c>
       <c r="BP11" t="n">
-        <v>-2.5</v>
+        <v>0.5</v>
       </c>
       <c r="BQ11" t="n">
-        <v>0.5</v>
+        <v>16.28509345794391</v>
+      </c>
+      <c r="BR11" t="n">
+        <v>2.616666666666667</v>
+      </c>
+      <c r="BS11" t="n">
+        <v>4.84788831288952</v>
       </c>
     </row>
     <row r="12">
@@ -2991,25 +3061,31 @@
         <v>22.35286640726341</v>
       </c>
       <c r="BK12" t="n">
-        <v>15.48730182926834</v>
+        <v>25.16593673965947</v>
       </c>
       <c r="BL12" t="n">
-        <v>25.16593673965947</v>
+        <v>3.833333333333333</v>
       </c>
       <c r="BM12" t="n">
-        <v>3.833333333333333</v>
+        <v>0.5899999999999999</v>
       </c>
       <c r="BN12" t="n">
-        <v>0.5899999999999999</v>
+        <v>4.399999999999999</v>
       </c>
       <c r="BO12" t="n">
-        <v>4.399999999999999</v>
+        <v>-3.109999999999999</v>
       </c>
       <c r="BP12" t="n">
-        <v>-3.109999999999999</v>
+        <v>3.100000000000001</v>
       </c>
       <c r="BQ12" t="n">
-        <v>3.100000000000001</v>
+        <v>15.45644376899704</v>
+      </c>
+      <c r="BR12" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="BS12" t="n">
+        <v>6.896422638266367</v>
       </c>
     </row>
     <row r="13">
@@ -3200,25 +3276,31 @@
         <v>17.81569230769247</v>
       </c>
       <c r="BK13" t="n">
-        <v>15.95729483282692</v>
+        <v>18.75245238095238</v>
       </c>
       <c r="BL13" t="n">
-        <v>18.75245238095238</v>
+        <v>21.2</v>
       </c>
       <c r="BM13" t="n">
-        <v>21.2</v>
+        <v>0.08999999999999986</v>
       </c>
       <c r="BN13" t="n">
-        <v>0.08999999999999986</v>
+        <v>0.5</v>
       </c>
       <c r="BO13" t="n">
-        <v>0.5</v>
+        <v>-1.609999999999999</v>
       </c>
       <c r="BP13" t="n">
-        <v>-1.609999999999999</v>
+        <v>-4.800000000000001</v>
       </c>
       <c r="BQ13" t="n">
-        <v>-4.800000000000001</v>
+        <v>16.20408194233684</v>
+      </c>
+      <c r="BR13" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS13" t="n">
+        <v>1.611610365355631</v>
       </c>
     </row>
     <row r="14">
@@ -3409,25 +3491,31 @@
         <v>18.76601282051293</v>
       </c>
       <c r="BK14" t="n">
-        <v>16.67735963581194</v>
+        <v>20.22346793349174</v>
       </c>
       <c r="BL14" t="n">
-        <v>20.22346793349174</v>
+        <v>8.816666666666666</v>
       </c>
       <c r="BM14" t="n">
-        <v>8.816666666666666</v>
+        <v>0.4000000000000004</v>
       </c>
       <c r="BN14" t="n">
-        <v>0.4000000000000004</v>
+        <v>6.59</v>
       </c>
       <c r="BO14" t="n">
-        <v>6.59</v>
+        <v>-2.199999999999999</v>
       </c>
       <c r="BP14" t="n">
-        <v>-2.199999999999999</v>
+        <v>-2.710000000000001</v>
       </c>
       <c r="BQ14" t="n">
-        <v>-2.710000000000001</v>
+        <v>17.13142640364192</v>
+      </c>
+      <c r="BR14" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS14" t="n">
+        <v>1.634586416871006</v>
       </c>
     </row>
     <row r="15">
@@ -3618,25 +3706,31 @@
         <v>20.70663252240734</v>
       </c>
       <c r="BK15" t="n">
-        <v>16.91737481031875</v>
+        <v>21.59638954869365</v>
       </c>
       <c r="BL15" t="n">
-        <v>21.59638954869365</v>
+        <v>0</v>
       </c>
       <c r="BM15" t="n">
-        <v>0</v>
+        <v>4.109999999999999</v>
       </c>
       <c r="BN15" t="n">
-        <v>4.109999999999999</v>
+        <v>1.609999999999999</v>
       </c>
       <c r="BO15" t="n">
-        <v>1.609999999999999</v>
+        <v>-0.9000000000000004</v>
       </c>
       <c r="BP15" t="n">
-        <v>-0.9000000000000004</v>
+        <v>-1.800000000000001</v>
       </c>
       <c r="BQ15" t="n">
-        <v>-1.800000000000001</v>
+        <v>15.88248861911995</v>
+      </c>
+      <c r="BR15" t="n">
+        <v>7.966666666666667</v>
+      </c>
+      <c r="BS15" t="n">
+        <v>4.824143903287393</v>
       </c>
     </row>
     <row r="16">
@@ -3827,25 +3921,31 @@
         <v>16.46234314980799</v>
       </c>
       <c r="BK16" t="n">
-        <v>15.24248861911992</v>
+        <v>16.99681710213779</v>
       </c>
       <c r="BL16" t="n">
-        <v>16.99681710213779</v>
+        <v>15.78333333333333</v>
       </c>
       <c r="BM16" t="n">
-        <v>15.78333333333333</v>
+        <v>0.3000000000000007</v>
       </c>
       <c r="BN16" t="n">
-        <v>0.3000000000000007</v>
+        <v>1.809999999999999</v>
       </c>
       <c r="BO16" t="n">
-        <v>1.809999999999999</v>
+        <v>-2</v>
       </c>
       <c r="BP16" t="n">
-        <v>-2</v>
+        <v>-3.800000000000001</v>
       </c>
       <c r="BQ16" t="n">
-        <v>-3.800000000000001</v>
+        <v>15.83864946889233</v>
+      </c>
+      <c r="BR16" t="n">
+        <v>0.8166666666666667</v>
+      </c>
+      <c r="BS16" t="n">
+        <v>0.623693680915661</v>
       </c>
     </row>
     <row r="17">
@@ -4036,25 +4136,31 @@
         <v>16.64960307298338</v>
       </c>
       <c r="BK17" t="n">
-        <v>15.27705614567533</v>
+        <v>16.40026128266035</v>
       </c>
       <c r="BL17" t="n">
-        <v>16.40026128266035</v>
+        <v>22.86666666666667</v>
       </c>
       <c r="BM17" t="n">
-        <v>22.86666666666667</v>
+        <v>0.2099999999999991</v>
       </c>
       <c r="BN17" t="n">
-        <v>0.2099999999999991</v>
+        <v>2.09</v>
       </c>
       <c r="BO17" t="n">
-        <v>2.09</v>
+        <v>-2.9</v>
       </c>
       <c r="BP17" t="n">
-        <v>-2.9</v>
+        <v>-4.399999999999999</v>
       </c>
       <c r="BQ17" t="n">
-        <v>-4.399999999999999</v>
+        <v>14.41911987860393</v>
+      </c>
+      <c r="BR17" t="n">
+        <v>4.016666666666667</v>
+      </c>
+      <c r="BS17" t="n">
+        <v>2.230483194379445</v>
       </c>
     </row>
     <row r="18">
@@ -4245,25 +4351,31 @@
         <v>17.14026957638006</v>
       </c>
       <c r="BK18" t="n">
-        <v>14.34892261001522</v>
+        <v>18.0260143198091</v>
       </c>
       <c r="BL18" t="n">
-        <v>18.0260143198091</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="BM18" t="n">
-        <v>8.699999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="BN18" t="n">
-        <v>0.5</v>
+        <v>1.41</v>
       </c>
       <c r="BO18" t="n">
-        <v>1.41</v>
+        <v>-2.31</v>
       </c>
       <c r="BP18" t="n">
-        <v>-2.31</v>
+        <v>-4.5</v>
       </c>
       <c r="BQ18" t="n">
-        <v>-4.5</v>
+        <v>13.96917933130703</v>
+      </c>
+      <c r="BR18" t="n">
+        <v>10.96666666666667</v>
+      </c>
+      <c r="BS18" t="n">
+        <v>3.171090245073035</v>
       </c>
     </row>
     <row r="19">
@@ -4454,25 +4566,31 @@
         <v>13.89230769230764</v>
       </c>
       <c r="BK19" t="n">
-        <v>13.14624048706245</v>
+        <v>13.91876484560576</v>
       </c>
       <c r="BL19" t="n">
-        <v>13.91876484560576</v>
+        <v>17.66666666666667</v>
       </c>
       <c r="BM19" t="n">
-        <v>17.66666666666667</v>
+        <v>0.5999999999999996</v>
       </c>
       <c r="BN19" t="n">
-        <v>0.5999999999999996</v>
+        <v>0.6099999999999994</v>
       </c>
       <c r="BO19" t="n">
-        <v>0.6099999999999994</v>
+        <v>-3.699999999999999</v>
       </c>
       <c r="BP19" t="n">
-        <v>-3.699999999999999</v>
+        <v>-8.609999999999999</v>
       </c>
       <c r="BQ19" t="n">
-        <v>-8.609999999999999</v>
+        <v>12.86922492401221</v>
+      </c>
+      <c r="BR19" t="n">
+        <v>5.85</v>
+      </c>
+      <c r="BS19" t="n">
+        <v>1.023082768295435</v>
       </c>
     </row>
     <row r="20">
@@ -4663,25 +4781,31 @@
         <v>17.6702816901409</v>
       </c>
       <c r="BK20" t="n">
-        <v>13.65330804248862</v>
+        <v>18.3416389548694</v>
       </c>
       <c r="BL20" t="n">
-        <v>18.3416389548694</v>
+        <v>8.716666666666667</v>
       </c>
       <c r="BM20" t="n">
-        <v>8.716666666666667</v>
+        <v>0.7099999999999991</v>
       </c>
       <c r="BN20" t="n">
-        <v>0.7099999999999991</v>
+        <v>1.09</v>
       </c>
       <c r="BO20" t="n">
-        <v>1.09</v>
+        <v>-3.609999999999999</v>
       </c>
       <c r="BP20" t="n">
-        <v>-3.609999999999999</v>
+        <v>-2.109999999999999</v>
       </c>
       <c r="BQ20" t="n">
-        <v>-2.109999999999999</v>
+        <v>13.8677996965099</v>
+      </c>
+      <c r="BR20" t="n">
+        <v>10.98333333333333</v>
+      </c>
+      <c r="BS20" t="n">
+        <v>3.802481993631005</v>
       </c>
     </row>
     <row r="21">
@@ -4872,25 +4996,31 @@
         <v>16.19034659820288</v>
       </c>
       <c r="BK21" t="n">
-        <v>13.89987841945291</v>
+        <v>17.05740476190479</v>
       </c>
       <c r="BL21" t="n">
-        <v>17.05740476190479</v>
+        <v>4.633333333333334</v>
       </c>
       <c r="BM21" t="n">
-        <v>4.633333333333334</v>
+        <v>1.41</v>
       </c>
       <c r="BN21" t="n">
-        <v>1.41</v>
+        <v>2.4</v>
       </c>
       <c r="BO21" t="n">
-        <v>2.4</v>
+        <v>-3.31</v>
       </c>
       <c r="BP21" t="n">
-        <v>-3.31</v>
+        <v>-5</v>
       </c>
       <c r="BQ21" t="n">
-        <v>-5</v>
+        <v>13.84667173252282</v>
+      </c>
+      <c r="BR21" t="n">
+        <v>10.96666666666667</v>
+      </c>
+      <c r="BS21" t="n">
+        <v>2.343674865680061</v>
       </c>
     </row>
     <row r="22">
@@ -5081,25 +5211,31 @@
         <v>17.42227912932147</v>
       </c>
       <c r="BK22" t="n">
-        <v>14.48103186646441</v>
+        <v>18.842541567696</v>
       </c>
       <c r="BL22" t="n">
-        <v>18.842541567696</v>
+        <v>4.2</v>
       </c>
       <c r="BM22" t="n">
-        <v>4.2</v>
+        <v>1.09</v>
       </c>
       <c r="BN22" t="n">
-        <v>1.09</v>
+        <v>1.790000000000001</v>
       </c>
       <c r="BO22" t="n">
-        <v>1.790000000000001</v>
+        <v>-3.31</v>
       </c>
       <c r="BP22" t="n">
-        <v>-3.31</v>
+        <v>-3.300000000000001</v>
       </c>
       <c r="BQ22" t="n">
-        <v>-3.300000000000001</v>
+        <v>15.45205167173263</v>
+      </c>
+      <c r="BR22" t="n">
+        <v>10.96666666666667</v>
+      </c>
+      <c r="BS22" t="n">
+        <v>1.970227457588841</v>
       </c>
     </row>
     <row r="23">
@@ -5290,25 +5426,31 @@
         <v>18.94521126760577</v>
       </c>
       <c r="BK23" t="n">
-        <v>15.9472796352584</v>
+        <v>21.43717339667464</v>
       </c>
       <c r="BL23" t="n">
-        <v>21.43717339667464</v>
+        <v>10.76666666666667</v>
       </c>
       <c r="BM23" t="n">
-        <v>10.76666666666667</v>
+        <v>0.2999999999999989</v>
       </c>
       <c r="BN23" t="n">
-        <v>0.2999999999999989</v>
+        <v>2.5</v>
       </c>
       <c r="BO23" t="n">
-        <v>2.5</v>
+        <v>-1.609999999999999</v>
       </c>
       <c r="BP23" t="n">
-        <v>-1.609999999999999</v>
+        <v>-0.5</v>
       </c>
       <c r="BQ23" t="n">
-        <v>-0.5</v>
+        <v>16.25084977238242</v>
+      </c>
+      <c r="BR23" t="n">
+        <v>10.38333333333333</v>
+      </c>
+      <c r="BS23" t="n">
+        <v>2.694361495223351</v>
       </c>
     </row>
     <row r="24">
@@ -5499,25 +5641,31 @@
         <v>19.25618437900144</v>
       </c>
       <c r="BK24" t="n">
-        <v>16.14585735963589</v>
+        <v>21.5853444180523</v>
       </c>
       <c r="BL24" t="n">
-        <v>21.5853444180523</v>
+        <v>12.3</v>
       </c>
       <c r="BM24" t="n">
-        <v>12.3</v>
+        <v>0.2099999999999991</v>
       </c>
       <c r="BN24" t="n">
-        <v>0.2099999999999991</v>
+        <v>2.5</v>
       </c>
       <c r="BO24" t="n">
-        <v>2.5</v>
+        <v>-1.109999999999999</v>
       </c>
       <c r="BP24" t="n">
         <v>-1.109999999999999</v>
       </c>
       <c r="BQ24" t="n">
-        <v>-1.109999999999999</v>
+        <v>15.28931714719273</v>
+      </c>
+      <c r="BR24" t="n">
+        <v>10.98333333333333</v>
+      </c>
+      <c r="BS24" t="n">
+        <v>3.966867231808711</v>
       </c>
     </row>
     <row r="25">
@@ -5708,25 +5856,31 @@
         <v>19.92505761843805</v>
       </c>
       <c r="BK25" t="n">
-        <v>14.90518968133545</v>
+        <v>22.02805225653209</v>
       </c>
       <c r="BL25" t="n">
-        <v>22.02805225653209</v>
+        <v>7.2</v>
       </c>
       <c r="BM25" t="n">
-        <v>7.2</v>
+        <v>0.2999999999999989</v>
       </c>
       <c r="BN25" t="n">
-        <v>0.2999999999999989</v>
+        <v>3.59</v>
       </c>
       <c r="BO25" t="n">
-        <v>3.59</v>
+        <v>-3.199999999999999</v>
       </c>
       <c r="BP25" t="n">
-        <v>-3.199999999999999</v>
+        <v>-1</v>
       </c>
       <c r="BQ25" t="n">
-        <v>-1</v>
+        <v>15.27095599393018</v>
+      </c>
+      <c r="BR25" t="n">
+        <v>10.98333333333333</v>
+      </c>
+      <c r="BS25" t="n">
+        <v>4.654101624507863</v>
       </c>
     </row>
     <row r="26">
@@ -5917,25 +6071,31 @@
         <v>20.54734274711181</v>
       </c>
       <c r="BK26" t="n">
-        <v>15.07241274658575</v>
+        <v>22.4577804295943</v>
       </c>
       <c r="BL26" t="n">
-        <v>22.4577804295943</v>
+        <v>13.15</v>
       </c>
       <c r="BM26" t="n">
-        <v>13.15</v>
+        <v>0.2900000000000009</v>
       </c>
       <c r="BN26" t="n">
-        <v>0.2900000000000009</v>
+        <v>4.81</v>
       </c>
       <c r="BO26" t="n">
-        <v>4.81</v>
+        <v>-2.4</v>
       </c>
       <c r="BP26" t="n">
-        <v>-2.4</v>
+        <v>-0.3999999999999986</v>
       </c>
       <c r="BQ26" t="n">
-        <v>-0.3999999999999986</v>
+        <v>15.41637329286812</v>
+      </c>
+      <c r="BR26" t="n">
+        <v>10.98333333333333</v>
+      </c>
+      <c r="BS26" t="n">
+        <v>5.130969454243681</v>
       </c>
     </row>
     <row r="27">
@@ -6126,25 +6286,31 @@
         <v>20.25357692307702</v>
       </c>
       <c r="BK27" t="n">
-        <v>15.0280880121396</v>
+        <v>22.48334916864615</v>
       </c>
       <c r="BL27" t="n">
-        <v>22.48334916864615</v>
+        <v>16.86666666666667</v>
       </c>
       <c r="BM27" t="n">
-        <v>16.86666666666667</v>
+        <v>0.2900000000000009</v>
       </c>
       <c r="BN27" t="n">
-        <v>0.2900000000000009</v>
+        <v>3.390000000000001</v>
       </c>
       <c r="BO27" t="n">
-        <v>3.390000000000001</v>
+        <v>-3.5</v>
       </c>
       <c r="BP27" t="n">
-        <v>-3.5</v>
+        <v>0.3900000000000006</v>
       </c>
       <c r="BQ27" t="n">
-        <v>0.3900000000000006</v>
+        <v>14.65984825493179</v>
+      </c>
+      <c r="BR27" t="n">
+        <v>0.3833333333333334</v>
+      </c>
+      <c r="BS27" t="n">
+        <v>5.593728668145234</v>
       </c>
     </row>
     <row r="28">
@@ -6335,25 +6501,31 @@
         <v>21.65866837387977</v>
       </c>
       <c r="BK28" t="n">
-        <v>14.56521276595745</v>
+        <v>23.85171021377682</v>
       </c>
       <c r="BL28" t="n">
-        <v>23.85171021377682</v>
+        <v>12.11666666666667</v>
       </c>
       <c r="BM28" t="n">
-        <v>12.11666666666667</v>
+        <v>0.7999999999999989</v>
       </c>
       <c r="BN28" t="n">
-        <v>0.7999999999999989</v>
+        <v>5.099999999999998</v>
       </c>
       <c r="BO28" t="n">
-        <v>5.099999999999998</v>
+        <v>-3.609999999999999</v>
       </c>
       <c r="BP28" t="n">
-        <v>-3.609999999999999</v>
+        <v>-0.3999999999999986</v>
       </c>
       <c r="BQ28" t="n">
-        <v>-0.3999999999999986</v>
+        <v>13.64753424657538</v>
+      </c>
+      <c r="BR28" t="n">
+        <v>5.333333333333333</v>
+      </c>
+      <c r="BS28" t="n">
+        <v>8.011134127304393</v>
       </c>
     </row>
     <row r="29">
@@ -6544,25 +6716,31 @@
         <v>21.39775641025654</v>
       </c>
       <c r="BK29" t="n">
-        <v>13.40496487119441</v>
+        <v>23.96952380952389</v>
       </c>
       <c r="BL29" t="n">
-        <v>23.96952380952389</v>
+        <v>8.866666666666667</v>
       </c>
       <c r="BM29" t="n">
-        <v>8.866666666666667</v>
+        <v>1.299999999999999</v>
       </c>
       <c r="BN29" t="n">
-        <v>1.299999999999999</v>
+        <v>4</v>
       </c>
       <c r="BO29" t="n">
-        <v>4</v>
+        <v>-3.81</v>
       </c>
       <c r="BP29" t="n">
-        <v>-3.81</v>
+        <v>0.7899999999999991</v>
       </c>
       <c r="BQ29" t="n">
-        <v>0.7899999999999991</v>
+        <v>13.7506775700935</v>
+      </c>
+      <c r="BR29" t="n">
+        <v>5.916666666666667</v>
+      </c>
+      <c r="BS29" t="n">
+        <v>7.647078840163042</v>
       </c>
     </row>
     <row r="30">
@@ -6753,25 +6931,31 @@
         <v>19.76014102564111</v>
       </c>
       <c r="BK30" t="n">
-        <v>14.51498480243163</v>
+        <v>22.01207142857151</v>
       </c>
       <c r="BL30" t="n">
-        <v>22.01207142857151</v>
+        <v>14.41666666666667</v>
       </c>
       <c r="BM30" t="n">
-        <v>14.41666666666667</v>
+        <v>1.31</v>
       </c>
       <c r="BN30" t="n">
-        <v>1.31</v>
+        <v>3.599999999999998</v>
       </c>
       <c r="BO30" t="n">
-        <v>3.599999999999998</v>
+        <v>-3.31</v>
       </c>
       <c r="BP30" t="n">
-        <v>-3.31</v>
+        <v>-2.5</v>
       </c>
       <c r="BQ30" t="n">
-        <v>-2.5</v>
+        <v>14.09015220700154</v>
+      </c>
+      <c r="BR30" t="n">
+        <v>0.2666666666666667</v>
+      </c>
+      <c r="BS30" t="n">
+        <v>5.669988818639567</v>
       </c>
     </row>
     <row r="31">
@@ -6962,25 +7146,31 @@
         <v>23.13428205128217</v>
       </c>
       <c r="BK31" t="n">
-        <v>14.04744680851067</v>
+        <v>25.83785714285728</v>
       </c>
       <c r="BL31" t="n">
-        <v>25.83785714285728</v>
+        <v>11.18333333333333</v>
       </c>
       <c r="BM31" t="n">
-        <v>11.18333333333333</v>
+        <v>0.7999999999999989</v>
       </c>
       <c r="BN31" t="n">
-        <v>0.7999999999999989</v>
+        <v>5.309999999999999</v>
       </c>
       <c r="BO31" t="n">
-        <v>5.309999999999999</v>
+        <v>-4.109999999999999</v>
       </c>
       <c r="BP31" t="n">
-        <v>-4.109999999999999</v>
+        <v>3.100000000000001</v>
       </c>
       <c r="BQ31" t="n">
-        <v>3.100000000000001</v>
+        <v>14.20526555386952</v>
+      </c>
+      <c r="BR31" t="n">
+        <v>1.816666666666667</v>
+      </c>
+      <c r="BS31" t="n">
+        <v>8.929016497412649</v>
       </c>
     </row>
     <row r="32">
@@ -7171,25 +7361,31 @@
         <v>23.56820282413365</v>
       </c>
       <c r="BK32" t="n">
-        <v>14.89790273556235</v>
+        <v>25.5159188544154</v>
       </c>
       <c r="BL32" t="n">
-        <v>25.5159188544154</v>
+        <v>10.56666666666667</v>
       </c>
       <c r="BM32" t="n">
-        <v>10.56666666666667</v>
+        <v>1.799999999999999</v>
       </c>
       <c r="BN32" t="n">
-        <v>1.799999999999999</v>
+        <v>4.690000000000001</v>
       </c>
       <c r="BO32" t="n">
-        <v>4.690000000000001</v>
+        <v>-3.699999999999999</v>
       </c>
       <c r="BP32" t="n">
-        <v>-3.699999999999999</v>
+        <v>3.289999999999999</v>
       </c>
       <c r="BQ32" t="n">
-        <v>3.289999999999999</v>
+        <v>16.98000000000011</v>
+      </c>
+      <c r="BR32" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="BS32" t="n">
+        <v>6.588202824133536</v>
       </c>
     </row>
     <row r="33">
@@ -7380,25 +7576,31 @@
         <v>17.10087067861726</v>
       </c>
       <c r="BK33" t="n">
-        <v>16.38676783004569</v>
+        <v>17.29237529691216</v>
       </c>
       <c r="BL33" t="n">
-        <v>17.29237529691216</v>
+        <v>5.583333333333333</v>
       </c>
       <c r="BM33" t="n">
-        <v>5.583333333333333</v>
+        <v>0.8900000000000006</v>
       </c>
       <c r="BN33" t="n">
-        <v>0.8900000000000006</v>
+        <v>2.500000000000002</v>
       </c>
       <c r="BO33" t="n">
-        <v>2.500000000000002</v>
+        <v>-0.9000000000000004</v>
       </c>
       <c r="BP33" t="n">
-        <v>-0.9000000000000004</v>
+        <v>-6.609999999999999</v>
       </c>
       <c r="BQ33" t="n">
-        <v>-6.609999999999999</v>
+        <v>15.46848024316111</v>
+      </c>
+      <c r="BR33" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS33" t="n">
+        <v>1.632390435456157</v>
       </c>
     </row>
     <row r="34">
@@ -7589,25 +7791,31 @@
         <v>14.72469910371322</v>
       </c>
       <c r="BK34" t="n">
-        <v>14.33217325227962</v>
+        <v>14.90489311163899</v>
       </c>
       <c r="BL34" t="n">
-        <v>14.90489311163899</v>
+        <v>0</v>
       </c>
       <c r="BM34" t="n">
-        <v>0</v>
+        <v>0.2900000000000009</v>
       </c>
       <c r="BN34" t="n">
-        <v>0.2900000000000009</v>
+        <v>1.200000000000001</v>
       </c>
       <c r="BO34" t="n">
-        <v>1.200000000000001</v>
+        <v>-3.5</v>
       </c>
       <c r="BP34" t="n">
-        <v>-3.5</v>
+        <v>-9.609999999999999</v>
       </c>
       <c r="BQ34" t="n">
-        <v>-9.609999999999999</v>
+        <v>13.95250379362678</v>
+      </c>
+      <c r="BR34" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS34" t="n">
+        <v>0.7721953100864347</v>
       </c>
     </row>
     <row r="35">
@@ -7798,25 +8006,31 @@
         <v>17.39989756722159</v>
       </c>
       <c r="BK35" t="n">
-        <v>14.6433232169955</v>
+        <v>18.01439429928745</v>
       </c>
       <c r="BL35" t="n">
-        <v>18.01439429928745</v>
+        <v>7.983333333333333</v>
       </c>
       <c r="BM35" t="n">
-        <v>7.983333333333333</v>
+        <v>0.08999999999999986</v>
       </c>
       <c r="BN35" t="n">
-        <v>0.08999999999999986</v>
+        <v>2.489999999999998</v>
       </c>
       <c r="BO35" t="n">
-        <v>2.489999999999998</v>
+        <v>-1.9</v>
       </c>
       <c r="BP35" t="n">
-        <v>-1.9</v>
+        <v>-4.109999999999999</v>
       </c>
       <c r="BQ35" t="n">
-        <v>-4.109999999999999</v>
+        <v>14.32415781487108</v>
+      </c>
+      <c r="BR35" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="BS35" t="n">
+        <v>3.075739752350504</v>
       </c>
     </row>
     <row r="36">
@@ -8007,25 +8221,31 @@
         <v>17.48427471116828</v>
       </c>
       <c r="BK36" t="n">
-        <v>14.22503058103977</v>
+        <v>19.06420427553447</v>
       </c>
       <c r="BL36" t="n">
-        <v>19.06420427553447</v>
+        <v>10.31666666666667</v>
       </c>
       <c r="BM36" t="n">
-        <v>10.31666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="BN36" t="n">
-        <v>0.5</v>
+        <v>4.210000000000001</v>
       </c>
       <c r="BO36" t="n">
-        <v>4.210000000000001</v>
+        <v>-3.199999999999999</v>
       </c>
       <c r="BP36" t="n">
-        <v>-3.199999999999999</v>
+        <v>-2.899999999999999</v>
       </c>
       <c r="BQ36" t="n">
-        <v>-2.899999999999999</v>
+        <v>13.87804281345568</v>
+      </c>
+      <c r="BR36" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="BS36" t="n">
+        <v>3.606231897712593</v>
       </c>
     </row>
     <row r="37">
@@ -8216,25 +8436,31 @@
         <v>19.8812724935734</v>
       </c>
       <c r="BK37" t="n">
-        <v>14.88100151745074</v>
+        <v>21.57155502392348</v>
       </c>
       <c r="BL37" t="n">
-        <v>21.57155502392348</v>
+        <v>4.366666666666666</v>
       </c>
       <c r="BM37" t="n">
-        <v>4.366666666666666</v>
+        <v>1.199999999999999</v>
       </c>
       <c r="BN37" t="n">
-        <v>1.199999999999999</v>
+        <v>2.300000000000001</v>
       </c>
       <c r="BO37" t="n">
-        <v>2.300000000000001</v>
+        <v>-3.699999999999999</v>
       </c>
       <c r="BP37" t="n">
-        <v>-3.699999999999999</v>
+        <v>-0.2100000000000009</v>
       </c>
       <c r="BQ37" t="n">
-        <v>-0.2100000000000009</v>
+        <v>15.97301972685888</v>
+      </c>
+      <c r="BR37" t="n">
+        <v>10.98333333333333</v>
+      </c>
+      <c r="BS37" t="n">
+        <v>3.908252766714522</v>
       </c>
     </row>
     <row r="38">
@@ -8425,25 +8651,31 @@
         <v>19.69882202304749</v>
       </c>
       <c r="BK38" t="n">
-        <v>15.05189681335362</v>
+        <v>21.54185273159153</v>
       </c>
       <c r="BL38" t="n">
-        <v>21.54185273159153</v>
+        <v>11.63333333333333</v>
       </c>
       <c r="BM38" t="n">
-        <v>11.63333333333333</v>
+        <v>0.7999999999999989</v>
       </c>
       <c r="BN38" t="n">
-        <v>0.7999999999999989</v>
+        <v>6.300000000000001</v>
       </c>
       <c r="BO38" t="n">
-        <v>6.300000000000001</v>
+        <v>-3.199999999999999</v>
       </c>
       <c r="BP38" t="n">
-        <v>-3.199999999999999</v>
+        <v>-2.800000000000001</v>
       </c>
       <c r="BQ38" t="n">
-        <v>-2.800000000000001</v>
+        <v>14.32197268588775</v>
+      </c>
+      <c r="BR38" t="n">
+        <v>10.98333333333333</v>
+      </c>
+      <c r="BS38" t="n">
+        <v>5.376849337159745</v>
       </c>
     </row>
     <row r="39">
@@ -8634,25 +8866,31 @@
         <v>23.20078305519906</v>
       </c>
       <c r="BK39" t="n">
-        <v>16.36851289833096</v>
+        <v>25.42114285714297</v>
       </c>
       <c r="BL39" t="n">
-        <v>25.42114285714297</v>
+        <v>6.133333333333334</v>
       </c>
       <c r="BM39" t="n">
-        <v>6.133333333333334</v>
+        <v>1.31</v>
       </c>
       <c r="BN39" t="n">
-        <v>1.31</v>
+        <v>2.5</v>
       </c>
       <c r="BO39" t="n">
-        <v>2.5</v>
+        <v>-3.31</v>
       </c>
       <c r="BP39" t="n">
-        <v>-3.31</v>
+        <v>3.199999999999999</v>
       </c>
       <c r="BQ39" t="n">
-        <v>3.199999999999999</v>
+        <v>18.1224734446131</v>
+      </c>
+      <c r="BR39" t="n">
+        <v>3.283333333333333</v>
+      </c>
+      <c r="BS39" t="n">
+        <v>5.078309610585958</v>
       </c>
     </row>
     <row r="40">
@@ -8843,25 +9081,31 @@
         <v>21.70816901408464</v>
       </c>
       <c r="BK40" t="n">
-        <v>16.3555538694994</v>
+        <v>23.48439429928749</v>
       </c>
       <c r="BL40" t="n">
-        <v>23.48439429928749</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="BM40" t="n">
-        <v>1.333333333333333</v>
+        <v>1.81</v>
       </c>
       <c r="BN40" t="n">
-        <v>1.81</v>
+        <v>6.199999999999999</v>
       </c>
       <c r="BO40" t="n">
-        <v>6.199999999999999</v>
+        <v>-2.81</v>
       </c>
       <c r="BP40" t="n">
-        <v>-2.81</v>
+        <v>0.6999999999999993</v>
       </c>
       <c r="BQ40" t="n">
-        <v>0.6999999999999993</v>
+        <v>15.24474962063734</v>
+      </c>
+      <c r="BR40" t="n">
+        <v>8.733333333333333</v>
+      </c>
+      <c r="BS40" t="n">
+        <v>6.463419393447303</v>
       </c>
     </row>
     <row r="41">
@@ -9052,25 +9296,31 @@
         <v>21.14930857874533</v>
       </c>
       <c r="BK41" t="n">
-        <v>14.48878603945376</v>
+        <v>23.50372921615209</v>
       </c>
       <c r="BL41" t="n">
-        <v>23.50372921615209</v>
+        <v>3.516666666666667</v>
       </c>
       <c r="BM41" t="n">
-        <v>3.516666666666667</v>
+        <v>0.5899999999999999</v>
       </c>
       <c r="BN41" t="n">
-        <v>0.5899999999999999</v>
+        <v>8.200000000000001</v>
       </c>
       <c r="BO41" t="n">
-        <v>8.200000000000001</v>
+        <v>-4.109999999999999</v>
       </c>
       <c r="BP41" t="n">
-        <v>-4.109999999999999</v>
+        <v>-0.1099999999999994</v>
       </c>
       <c r="BQ41" t="n">
-        <v>-0.1099999999999994</v>
+        <v>13.76599383667186</v>
+      </c>
+      <c r="BR41" t="n">
+        <v>9.483333333333333</v>
+      </c>
+      <c r="BS41" t="n">
+        <v>7.383314742073475</v>
       </c>
     </row>
     <row r="42">
@@ -9261,25 +9511,31 @@
         <v>19.05614395886901</v>
       </c>
       <c r="BK42" t="n">
-        <v>14.70930555555561</v>
+        <v>20.63770334928236</v>
       </c>
       <c r="BL42" t="n">
-        <v>20.63770334928236</v>
+        <v>1.15</v>
       </c>
       <c r="BM42" t="n">
-        <v>1.15</v>
+        <v>1</v>
       </c>
       <c r="BN42" t="n">
-        <v>1</v>
+        <v>2.900000000000002</v>
       </c>
       <c r="BO42" t="n">
-        <v>2.900000000000002</v>
+        <v>-3.81</v>
       </c>
       <c r="BP42" t="n">
-        <v>-3.81</v>
+        <v>-3.399999999999999</v>
       </c>
       <c r="BQ42" t="n">
-        <v>-3.399999999999999</v>
+        <v>14.56762658227856</v>
+      </c>
+      <c r="BR42" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="BS42" t="n">
+        <v>4.488517376590446</v>
       </c>
     </row>
     <row r="43">
@@ -9470,25 +9726,31 @@
         <v>14.94691025641034</v>
       </c>
       <c r="BK43" t="n">
-        <v>13.77962085308062</v>
+        <v>15.45223809523813</v>
       </c>
       <c r="BL43" t="n">
-        <v>15.45223809523813</v>
+        <v>7.583333333333333</v>
       </c>
       <c r="BM43" t="n">
-        <v>7.583333333333333</v>
+        <v>3.209999999999999</v>
       </c>
       <c r="BN43" t="n">
-        <v>3.209999999999999</v>
+        <v>1.1</v>
       </c>
       <c r="BO43" t="n">
-        <v>1.1</v>
+        <v>-4.609999999999999</v>
       </c>
       <c r="BP43" t="n">
-        <v>-4.609999999999999</v>
+        <v>-7.710000000000001</v>
       </c>
       <c r="BQ43" t="n">
-        <v>-7.710000000000001</v>
+        <v>14.14383915022765</v>
+      </c>
+      <c r="BR43" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="BS43" t="n">
+        <v>0.8030711061826956</v>
       </c>
     </row>
     <row r="44">
@@ -9679,25 +9941,31 @@
         <v>18.30852374839545</v>
       </c>
       <c r="BK44" t="n">
-        <v>14.37408194233689</v>
+        <v>18.66138424821007</v>
       </c>
       <c r="BL44" t="n">
-        <v>18.66138424821007</v>
+        <v>14.35</v>
       </c>
       <c r="BM44" t="n">
-        <v>14.35</v>
+        <v>0.5</v>
       </c>
       <c r="BN44" t="n">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="BO44" t="n">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="BP44" t="n">
-        <v>-3</v>
+        <v>-2.210000000000001</v>
       </c>
       <c r="BQ44" t="n">
-        <v>-2.210000000000001</v>
+        <v>14.39303951367785</v>
+      </c>
+      <c r="BR44" t="n">
+        <v>10.96666666666667</v>
+      </c>
+      <c r="BS44" t="n">
+        <v>3.915484234717599</v>
       </c>
     </row>
     <row r="45">
@@ -9888,25 +10156,31 @@
         <v>19.20761538461556</v>
       </c>
       <c r="BK45" t="n">
-        <v>14.18351063829791</v>
+        <v>20.73978622327793</v>
       </c>
       <c r="BL45" t="n">
-        <v>20.73978622327793</v>
+        <v>9.483333333333333</v>
       </c>
       <c r="BM45" t="n">
-        <v>9.483333333333333</v>
+        <v>0.7099999999999991</v>
       </c>
       <c r="BN45" t="n">
-        <v>0.7099999999999991</v>
+        <v>4.899999999999999</v>
       </c>
       <c r="BO45" t="n">
-        <v>4.899999999999999</v>
+        <v>-2.699999999999999</v>
       </c>
       <c r="BP45" t="n">
-        <v>-2.699999999999999</v>
+        <v>-2.210000000000001</v>
       </c>
       <c r="BQ45" t="n">
-        <v>-2.210000000000001</v>
+        <v>13.40549317147196</v>
+      </c>
+      <c r="BR45" t="n">
+        <v>9.016666666666667</v>
+      </c>
+      <c r="BS45" t="n">
+        <v>5.802122213143601</v>
       </c>
     </row>
     <row r="46">
@@ -10097,25 +10371,31 @@
         <v>20.96393316195385</v>
       </c>
       <c r="BK46" t="n">
-        <v>13.33896499238968</v>
+        <v>23.10582338902158</v>
       </c>
       <c r="BL46" t="n">
-        <v>23.10582338902158</v>
+        <v>10.76666666666667</v>
       </c>
       <c r="BM46" t="n">
-        <v>10.76666666666667</v>
+        <v>0.8100000000000005</v>
       </c>
       <c r="BN46" t="n">
-        <v>0.8100000000000005</v>
+        <v>5.289999999999999</v>
       </c>
       <c r="BO46" t="n">
-        <v>5.289999999999999</v>
+        <v>-4.109999999999999</v>
       </c>
       <c r="BP46" t="n">
-        <v>-4.109999999999999</v>
+        <v>0.3900000000000006</v>
       </c>
       <c r="BQ46" t="n">
-        <v>0.3900000000000006</v>
+        <v>14.09295558958655</v>
+      </c>
+      <c r="BR46" t="n">
+        <v>9.35</v>
+      </c>
+      <c r="BS46" t="n">
+        <v>6.870977572367302</v>
       </c>
     </row>
     <row r="47">
@@ -10306,25 +10586,31 @@
         <v>20.63720154043661</v>
       </c>
       <c r="BK47" t="n">
-        <v>14.08584732824432</v>
+        <v>22.4965714285715</v>
       </c>
       <c r="BL47" t="n">
-        <v>22.4965714285715</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="BM47" t="n">
-        <v>0.5666666666666667</v>
+        <v>0.7099999999999991</v>
       </c>
       <c r="BN47" t="n">
-        <v>0.7099999999999991</v>
+        <v>5.300000000000001</v>
       </c>
       <c r="BO47" t="n">
-        <v>5.300000000000001</v>
+        <v>-3.5</v>
       </c>
       <c r="BP47" t="n">
-        <v>-3.5</v>
+        <v>-0.2100000000000009</v>
       </c>
       <c r="BQ47" t="n">
-        <v>-0.2100000000000009</v>
+        <v>14.48669195751141</v>
+      </c>
+      <c r="BR47" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="BS47" t="n">
+        <v>6.150509582925208</v>
       </c>
     </row>
     <row r="48">
@@ -10515,25 +10801,31 @@
         <v>21.66891025641041</v>
       </c>
       <c r="BK48" t="n">
-        <v>14.72396054628229</v>
+        <v>24.20702380952389</v>
       </c>
       <c r="BL48" t="n">
-        <v>24.20702380952389</v>
+        <v>4.95</v>
       </c>
       <c r="BM48" t="n">
-        <v>4.95</v>
+        <v>1.31</v>
       </c>
       <c r="BN48" t="n">
-        <v>1.31</v>
+        <v>6.809999999999999</v>
       </c>
       <c r="BO48" t="n">
-        <v>6.809999999999999</v>
+        <v>-3.31</v>
       </c>
       <c r="BP48" t="n">
-        <v>-3.31</v>
+        <v>0.1999999999999993</v>
       </c>
       <c r="BQ48" t="n">
-        <v>0.1999999999999993</v>
+        <v>13.98106221547805</v>
+      </c>
+      <c r="BR48" t="n">
+        <v>10.01666666666667</v>
+      </c>
+      <c r="BS48" t="n">
+        <v>7.687848040932357</v>
       </c>
     </row>
     <row r="49">
@@ -10724,25 +11016,31 @@
         <v>25.1845838668375</v>
       </c>
       <c r="BK49" t="n">
-        <v>14.74344984802432</v>
+        <v>28.87980997624718</v>
       </c>
       <c r="BL49" t="n">
-        <v>28.87980997624718</v>
+        <v>9.6</v>
       </c>
       <c r="BM49" t="n">
-        <v>9.6</v>
+        <v>1.110000000000001</v>
       </c>
       <c r="BN49" t="n">
-        <v>1.110000000000001</v>
+        <v>7.399999999999999</v>
       </c>
       <c r="BO49" t="n">
-        <v>7.399999999999999</v>
+        <v>-3.4</v>
       </c>
       <c r="BP49" t="n">
-        <v>-3.4</v>
+        <v>5.890000000000001</v>
       </c>
       <c r="BQ49" t="n">
-        <v>5.890000000000001</v>
+        <v>15.10103343465049</v>
+      </c>
+      <c r="BR49" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="BS49" t="n">
+        <v>10.08355043218702</v>
       </c>
     </row>
     <row r="50">
@@ -10933,25 +11231,31 @@
         <v>24.47288461538473</v>
       </c>
       <c r="BK50" t="n">
-        <v>14.71907435508347</v>
+        <v>27.05102137767233</v>
       </c>
       <c r="BL50" t="n">
-        <v>27.05102137767233</v>
+        <v>12.45</v>
       </c>
       <c r="BM50" t="n">
-        <v>12.45</v>
+        <v>1</v>
       </c>
       <c r="BN50" t="n">
-        <v>1</v>
+        <v>5.689999999999998</v>
       </c>
       <c r="BO50" t="n">
-        <v>5.689999999999998</v>
+        <v>-3.699999999999999</v>
       </c>
       <c r="BP50" t="n">
-        <v>-3.699999999999999</v>
+        <v>5.600000000000001</v>
       </c>
       <c r="BQ50" t="n">
-        <v>5.600000000000001</v>
+        <v>15.05001517450681</v>
+      </c>
+      <c r="BR50" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="BS50" t="n">
+        <v>9.422869440877912</v>
       </c>
     </row>
     <row r="51">
@@ -11142,25 +11446,31 @@
         <v>20.39829048843199</v>
       </c>
       <c r="BK51" t="n">
-        <v>16.71575113808807</v>
+        <v>22.93318181818191</v>
       </c>
       <c r="BL51" t="n">
-        <v>22.93318181818191</v>
+        <v>9.916666666666666</v>
       </c>
       <c r="BM51" t="n">
-        <v>9.916666666666666</v>
+        <v>1.59</v>
       </c>
       <c r="BN51" t="n">
-        <v>1.59</v>
+        <v>1.5</v>
       </c>
       <c r="BO51" t="n">
-        <v>1.5</v>
+        <v>-2.81</v>
       </c>
       <c r="BP51" t="n">
-        <v>-2.81</v>
+        <v>0</v>
       </c>
       <c r="BQ51" t="n">
-        <v>0</v>
+        <v>17.25875379939212</v>
+      </c>
+      <c r="BR51" t="n">
+        <v>1.883333333333333</v>
+      </c>
+      <c r="BS51" t="n">
+        <v>3.139536689039868</v>
       </c>
     </row>
     <row r="52">
@@ -11351,25 +11661,31 @@
         <v>16.0976440460948</v>
       </c>
       <c r="BK52" t="n">
-        <v>15.12892097264436</v>
+        <v>15.84137767220899</v>
       </c>
       <c r="BL52" t="n">
-        <v>15.84137767220899</v>
+        <v>0</v>
       </c>
       <c r="BM52" t="n">
-        <v>0</v>
+        <v>0.4000000000000004</v>
       </c>
       <c r="BN52" t="n">
-        <v>0.4000000000000004</v>
+        <v>0.4100000000000001</v>
       </c>
       <c r="BO52" t="n">
-        <v>0.4100000000000001</v>
+        <v>-1.699999999999999</v>
       </c>
       <c r="BP52" t="n">
-        <v>-1.699999999999999</v>
+        <v>-6.609999999999999</v>
       </c>
       <c r="BQ52" t="n">
-        <v>-6.609999999999999</v>
+        <v>14.34077389984826</v>
+      </c>
+      <c r="BR52" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS52" t="n">
+        <v>1.756870146246541</v>
       </c>
     </row>
     <row r="53">
@@ -11560,25 +11876,31 @@
         <v>18.29252564102573</v>
       </c>
       <c r="BK53" t="n">
-        <v>15.08464339908955</v>
+        <v>19.26315914489315</v>
       </c>
       <c r="BL53" t="n">
-        <v>19.26315914489315</v>
+        <v>7.033333333333333</v>
       </c>
       <c r="BM53" t="n">
-        <v>7.033333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="BN53" t="n">
-        <v>0.5</v>
+        <v>1.41</v>
       </c>
       <c r="BO53" t="n">
-        <v>1.41</v>
+        <v>-2.199999999999999</v>
       </c>
       <c r="BP53" t="n">
-        <v>-2.199999999999999</v>
+        <v>-4.300000000000001</v>
       </c>
       <c r="BQ53" t="n">
-        <v>-4.300000000000001</v>
+        <v>14.26418816388472</v>
+      </c>
+      <c r="BR53" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS53" t="n">
+        <v>4.028337477141015</v>
       </c>
     </row>
     <row r="54">
@@ -11769,25 +12091,31 @@
         <v>22.03661538461554</v>
       </c>
       <c r="BK54" t="n">
-        <v>13.60878603945373</v>
+        <v>24.56266033254166</v>
       </c>
       <c r="BL54" t="n">
-        <v>24.56266033254166</v>
+        <v>7.066666666666666</v>
       </c>
       <c r="BM54" t="n">
-        <v>7.066666666666666</v>
+        <v>1.799999999999999</v>
       </c>
       <c r="BN54" t="n">
-        <v>1.799999999999999</v>
+        <v>6.699999999999999</v>
       </c>
       <c r="BO54" t="n">
-        <v>6.699999999999999</v>
+        <v>-4.609999999999999</v>
       </c>
       <c r="BP54" t="n">
-        <v>-4.609999999999999</v>
+        <v>1</v>
       </c>
       <c r="BQ54" t="n">
-        <v>1</v>
+        <v>14.55830534351151</v>
+      </c>
+      <c r="BR54" t="n">
+        <v>4.466666666666667</v>
+      </c>
+      <c r="BS54" t="n">
+        <v>7.478310041104038</v>
       </c>
     </row>
     <row r="55">
@@ -11978,25 +12306,31 @@
         <v>21.57476562500013</v>
       </c>
       <c r="BK55" t="n">
-        <v>14.49654961832063</v>
+        <v>24.03665083135402</v>
       </c>
       <c r="BL55" t="n">
-        <v>24.03665083135402</v>
+        <v>12.51666666666667</v>
       </c>
       <c r="BM55" t="n">
-        <v>12.51666666666667</v>
+        <v>0.7999999999999989</v>
       </c>
       <c r="BN55" t="n">
-        <v>0.7999999999999989</v>
+        <v>7.1</v>
       </c>
       <c r="BO55" t="n">
-        <v>7.1</v>
+        <v>-2.699999999999999</v>
       </c>
       <c r="BP55" t="n">
-        <v>-2.699999999999999</v>
+        <v>0.1999999999999993</v>
       </c>
       <c r="BQ55" t="n">
-        <v>0.1999999999999993</v>
+        <v>14.79068285280732</v>
+      </c>
+      <c r="BR55" t="n">
+        <v>8.833333333333334</v>
+      </c>
+      <c r="BS55" t="n">
+        <v>6.784082772192807</v>
       </c>
     </row>
     <row r="56">
@@ -12187,25 +12521,31 @@
         <v>21.39399487836123</v>
       </c>
       <c r="BK56" t="n">
-        <v>14.653808801214</v>
+        <v>23.79453681710222</v>
       </c>
       <c r="BL56" t="n">
-        <v>23.79453681710222</v>
+        <v>6.433333333333334</v>
       </c>
       <c r="BM56" t="n">
-        <v>6.433333333333334</v>
+        <v>0.7000000000000011</v>
       </c>
       <c r="BN56" t="n">
-        <v>0.7000000000000011</v>
+        <v>4.5</v>
       </c>
       <c r="BO56" t="n">
-        <v>4.5</v>
+        <v>-3.81</v>
       </c>
       <c r="BP56" t="n">
-        <v>-3.81</v>
+        <v>0</v>
       </c>
       <c r="BQ56" t="n">
-        <v>0</v>
+        <v>14.26689969604866</v>
+      </c>
+      <c r="BR56" t="n">
+        <v>1.783333333333333</v>
+      </c>
+      <c r="BS56" t="n">
+        <v>7.127095182312578</v>
       </c>
     </row>
     <row r="57">
@@ -12396,25 +12736,31 @@
         <v>21.93107554417429</v>
       </c>
       <c r="BK57" t="n">
-        <v>14.91268996960487</v>
+        <v>24.4562945368172</v>
       </c>
       <c r="BL57" t="n">
-        <v>24.4562945368172</v>
+        <v>9.383333333333333</v>
       </c>
       <c r="BM57" t="n">
-        <v>9.383333333333333</v>
+        <v>5.710000000000001</v>
       </c>
       <c r="BN57" t="n">
-        <v>5.710000000000001</v>
+        <v>6.099999999999998</v>
       </c>
       <c r="BO57" t="n">
-        <v>6.099999999999998</v>
+        <v>-5.5</v>
       </c>
       <c r="BP57" t="n">
-        <v>-5.5</v>
+        <v>0.5</v>
       </c>
       <c r="BQ57" t="n">
-        <v>0.5</v>
+        <v>15.47995447647953</v>
+      </c>
+      <c r="BR57" t="n">
+        <v>10.53333333333333</v>
+      </c>
+      <c r="BS57" t="n">
+        <v>6.451121067694753</v>
       </c>
     </row>
     <row r="58">
@@ -12605,25 +12951,31 @@
         <v>22.77199743918065</v>
       </c>
       <c r="BK58" t="n">
-        <v>15.27710166919576</v>
+        <v>25.59942992874116</v>
       </c>
       <c r="BL58" t="n">
-        <v>25.59942992874116</v>
+        <v>5.316666666666666</v>
       </c>
       <c r="BM58" t="n">
-        <v>5.316666666666666</v>
+        <v>0.7999999999999989</v>
       </c>
       <c r="BN58" t="n">
-        <v>0.7999999999999989</v>
+        <v>5.5</v>
       </c>
       <c r="BO58" t="n">
-        <v>5.5</v>
+        <v>-2.609999999999999</v>
       </c>
       <c r="BP58" t="n">
-        <v>-2.609999999999999</v>
+        <v>2.600000000000001</v>
       </c>
       <c r="BQ58" t="n">
-        <v>2.600000000000001</v>
+        <v>15.0179969650986</v>
+      </c>
+      <c r="BR58" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="BS58" t="n">
+        <v>7.75400047408205</v>
       </c>
     </row>
     <row r="59">
@@ -12814,25 +13166,31 @@
         <v>24.78533930857884</v>
       </c>
       <c r="BK59" t="n">
-        <v>17.30199088145906</v>
+        <v>27.24315914489319</v>
       </c>
       <c r="BL59" t="n">
-        <v>27.24315914489319</v>
+        <v>5.1</v>
       </c>
       <c r="BM59" t="n">
-        <v>5.1</v>
+        <v>1.9</v>
       </c>
       <c r="BN59" t="n">
-        <v>1.9</v>
+        <v>4.100000000000001</v>
       </c>
       <c r="BO59" t="n">
-        <v>4.100000000000001</v>
+        <v>-2.109999999999999</v>
       </c>
       <c r="BP59" t="n">
-        <v>-2.109999999999999</v>
+        <v>3.699999999999999</v>
       </c>
       <c r="BQ59" t="n">
-        <v>3.699999999999999</v>
+        <v>18.83951367781164</v>
+      </c>
+      <c r="BR59" t="n">
+        <v>1</v>
+      </c>
+      <c r="BS59" t="n">
+        <v>5.945825630767199</v>
       </c>
     </row>
     <row r="60">
@@ -13023,25 +13381,31 @@
         <v>24.97378690629024</v>
       </c>
       <c r="BK60" t="n">
-        <v>19.25663125948414</v>
+        <v>26.87250596658722</v>
       </c>
       <c r="BL60" t="n">
-        <v>26.87250596658722</v>
+        <v>6.983333333333333</v>
       </c>
       <c r="BM60" t="n">
-        <v>6.983333333333333</v>
+        <v>1.81</v>
       </c>
       <c r="BN60" t="n">
-        <v>1.81</v>
+        <v>2.189999999999998</v>
       </c>
       <c r="BO60" t="n">
-        <v>2.189999999999998</v>
+        <v>-0.3100000000000005</v>
       </c>
       <c r="BP60" t="n">
-        <v>-0.3100000000000005</v>
+        <v>3.890000000000001</v>
       </c>
       <c r="BQ60" t="n">
-        <v>3.890000000000001</v>
+        <v>20.27308980213105</v>
+      </c>
+      <c r="BR60" t="n">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="BS60" t="n">
+        <v>4.70069710415919</v>
       </c>
     </row>
     <row r="61">
@@ -13232,25 +13596,31 @@
         <v>21.87734955185669</v>
       </c>
       <c r="BK61" t="n">
-        <v>17.67462709284625</v>
+        <v>21.28425178147275</v>
       </c>
       <c r="BL61" t="n">
-        <v>21.28425178147275</v>
+        <v>5.283333333333333</v>
       </c>
       <c r="BM61" t="n">
-        <v>5.283333333333333</v>
+        <v>0.8000000000000007</v>
       </c>
       <c r="BN61" t="n">
-        <v>0.8000000000000007</v>
+        <v>1.699999999999999</v>
       </c>
       <c r="BO61" t="n">
-        <v>1.699999999999999</v>
+        <v>-1.5</v>
       </c>
       <c r="BP61" t="n">
-        <v>-1.5</v>
+        <v>3.199999999999999</v>
       </c>
       <c r="BQ61" t="n">
-        <v>3.199999999999999</v>
+        <v>14.77113808801217</v>
+      </c>
+      <c r="BR61" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS61" t="n">
+        <v>7.106211463844522</v>
       </c>
     </row>
     <row r="62">
@@ -13441,25 +13811,31 @@
         <v>19.31746478873252</v>
       </c>
       <c r="BK62" t="n">
-        <v>13.97799696509867</v>
+        <v>19.88182897862236</v>
       </c>
       <c r="BL62" t="n">
-        <v>19.88182897862236</v>
+        <v>4.8</v>
       </c>
       <c r="BM62" t="n">
-        <v>4.8</v>
+        <v>1</v>
       </c>
       <c r="BN62" t="n">
-        <v>1</v>
+        <v>5.199999999999999</v>
       </c>
       <c r="BO62" t="n">
-        <v>5.199999999999999</v>
+        <v>-4.31</v>
       </c>
       <c r="BP62" t="n">
-        <v>-4.31</v>
+        <v>-3.899999999999999</v>
       </c>
       <c r="BQ62" t="n">
-        <v>-3.899999999999999</v>
+        <v>13.96793626707135</v>
+      </c>
+      <c r="BR62" t="n">
+        <v>3.116666666666667</v>
+      </c>
+      <c r="BS62" t="n">
+        <v>5.349528521661169</v>
       </c>
     </row>
     <row r="63">
@@ -13650,25 +14026,31 @@
         <v>21.69035851472487</v>
       </c>
       <c r="BK63" t="n">
-        <v>14.40464339908955</v>
+        <v>23.02909738717346</v>
       </c>
       <c r="BL63" t="n">
-        <v>23.02909738717346</v>
+        <v>9.566666666666666</v>
       </c>
       <c r="BM63" t="n">
-        <v>9.566666666666666</v>
+        <v>4.200000000000001</v>
       </c>
       <c r="BN63" t="n">
-        <v>4.200000000000001</v>
+        <v>5.899999999999999</v>
       </c>
       <c r="BO63" t="n">
-        <v>5.899999999999999</v>
+        <v>-4.9</v>
       </c>
       <c r="BP63" t="n">
-        <v>-4.9</v>
+        <v>-0.6099999999999994</v>
       </c>
       <c r="BQ63" t="n">
-        <v>-0.6099999999999994</v>
+        <v>14.50423368740519</v>
+      </c>
+      <c r="BR63" t="n">
+        <v>5.866666666666666</v>
+      </c>
+      <c r="BS63" t="n">
+        <v>7.186124827319686</v>
       </c>
     </row>
     <row r="64">
@@ -13859,25 +14241,31 @@
         <v>23.68670934699115</v>
       </c>
       <c r="BK64" t="n">
-        <v>16.81596358118371</v>
+        <v>26.18320665083145</v>
       </c>
       <c r="BL64" t="n">
-        <v>26.18320665083145</v>
+        <v>10.98333333333333</v>
       </c>
       <c r="BM64" t="n">
-        <v>10.98333333333333</v>
+        <v>1.199999999999999</v>
       </c>
       <c r="BN64" t="n">
-        <v>1.199999999999999</v>
+        <v>3.789999999999999</v>
       </c>
       <c r="BO64" t="n">
-        <v>3.789999999999999</v>
+        <v>-2.699999999999999</v>
       </c>
       <c r="BP64" t="n">
-        <v>-2.699999999999999</v>
+        <v>3.100000000000001</v>
       </c>
       <c r="BQ64" t="n">
-        <v>3.100000000000001</v>
+        <v>18.61624620060811</v>
+      </c>
+      <c r="BR64" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="BS64" t="n">
+        <v>5.070463146383041</v>
       </c>
     </row>
     <row r="65">
@@ -14068,25 +14456,31 @@
         <v>19.07671373555851</v>
       </c>
       <c r="BK65" t="n">
-        <v>17.7083282674773</v>
+        <v>19.75447619047624</v>
       </c>
       <c r="BL65" t="n">
-        <v>19.75447619047624</v>
+        <v>1.1</v>
       </c>
       <c r="BM65" t="n">
-        <v>1.1</v>
+        <v>0.1899999999999977</v>
       </c>
       <c r="BN65" t="n">
-        <v>0.1899999999999977</v>
+        <v>0.7100000000000009</v>
       </c>
       <c r="BO65" t="n">
-        <v>0.7100000000000009</v>
+        <v>1</v>
       </c>
       <c r="BP65" t="n">
-        <v>1</v>
+        <v>-4.710000000000001</v>
       </c>
       <c r="BQ65" t="n">
-        <v>-4.710000000000001</v>
+        <v>17.71966616084976</v>
+      </c>
+      <c r="BR65" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS65" t="n">
+        <v>1.357047574708748</v>
       </c>
     </row>
     <row r="66">
@@ -14277,25 +14671,31 @@
         <v>21.35648648648662</v>
       </c>
       <c r="BK66" t="n">
-        <v>17.27071320182096</v>
+        <v>23.72938242280292</v>
       </c>
       <c r="BL66" t="n">
-        <v>23.72938242280292</v>
+        <v>4.933333333333334</v>
       </c>
       <c r="BM66" t="n">
-        <v>4.933333333333334</v>
+        <v>0.3000000000000007</v>
       </c>
       <c r="BN66" t="n">
-        <v>0.3000000000000007</v>
+        <v>5.5</v>
       </c>
       <c r="BO66" t="n">
-        <v>5.5</v>
+        <v>-1.609999999999999</v>
       </c>
       <c r="BP66" t="n">
-        <v>-1.609999999999999</v>
+        <v>0.1999999999999993</v>
       </c>
       <c r="BQ66" t="n">
-        <v>0.1999999999999993</v>
+        <v>15.64107902735571</v>
+      </c>
+      <c r="BR66" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS66" t="n">
+        <v>5.715407459130914</v>
       </c>
     </row>
     <row r="67">
@@ -14486,25 +14886,31 @@
         <v>22.52345806451625</v>
       </c>
       <c r="BK67" t="n">
-        <v>15.32640791476411</v>
+        <v>24.79245783132537</v>
       </c>
       <c r="BL67" t="n">
-        <v>24.79245783132537</v>
+        <v>5.583333333333333</v>
       </c>
       <c r="BM67" t="n">
-        <v>5.583333333333333</v>
+        <v>1.600000000000001</v>
       </c>
       <c r="BN67" t="n">
-        <v>1.600000000000001</v>
+        <v>5.399999999999999</v>
       </c>
       <c r="BO67" t="n">
-        <v>5.399999999999999</v>
+        <v>-2.199999999999999</v>
       </c>
       <c r="BP67" t="n">
-        <v>-2.199999999999999</v>
+        <v>0.7899999999999991</v>
       </c>
       <c r="BQ67" t="n">
-        <v>0.7899999999999991</v>
+        <v>14.04132218844986</v>
+      </c>
+      <c r="BR67" t="n">
+        <v>3.316666666666667</v>
+      </c>
+      <c r="BS67" t="n">
+        <v>8.482135876066389</v>
       </c>
     </row>
     <row r="68">
@@ -14695,25 +15101,31 @@
         <v>22.00193341869415</v>
       </c>
       <c r="BK68" t="n">
-        <v>13.7099696509864</v>
+        <v>24.14220902612836</v>
       </c>
       <c r="BL68" t="n">
-        <v>24.14220902612836</v>
+        <v>1.566666666666667</v>
       </c>
       <c r="BM68" t="n">
-        <v>1.566666666666667</v>
+        <v>4.200000000000001</v>
       </c>
       <c r="BN68" t="n">
-        <v>4.200000000000001</v>
+        <v>5.289999999999999</v>
       </c>
       <c r="BO68" t="n">
-        <v>5.289999999999999</v>
+        <v>-5.31</v>
       </c>
       <c r="BP68" t="n">
-        <v>-5.31</v>
+        <v>-0.3999999999999986</v>
       </c>
       <c r="BQ68" t="n">
-        <v>-0.3999999999999986</v>
+        <v>13.90861911987864</v>
+      </c>
+      <c r="BR68" t="n">
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="BS68" t="n">
+        <v>8.093314298815512</v>
       </c>
     </row>
     <row r="69">
@@ -14904,25 +15316,31 @@
         <v>21.50754161331643</v>
       </c>
       <c r="BK69" t="n">
-        <v>13.77477996965103</v>
+        <v>24.02121140142528</v>
       </c>
       <c r="BL69" t="n">
-        <v>24.02121140142528</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="BM69" t="n">
-        <v>3.333333333333333</v>
+        <v>3.299999999999999</v>
       </c>
       <c r="BN69" t="n">
-        <v>3.299999999999999</v>
+        <v>6</v>
       </c>
       <c r="BO69" t="n">
-        <v>6</v>
+        <v>-4.199999999999999</v>
       </c>
       <c r="BP69" t="n">
-        <v>-4.199999999999999</v>
+        <v>-0.1099999999999994</v>
       </c>
       <c r="BQ69" t="n">
-        <v>-0.1099999999999994</v>
+        <v>14.93772382397565</v>
+      </c>
+      <c r="BR69" t="n">
+        <v>0.8166666666666667</v>
+      </c>
+      <c r="BS69" t="n">
+        <v>6.569817789340782</v>
       </c>
     </row>
     <row r="70">
@@ -15113,25 +15531,31 @@
         <v>21.9294993581516</v>
       </c>
       <c r="BK70" t="n">
-        <v>16.02959028831576</v>
+        <v>24.67541766109792</v>
       </c>
       <c r="BL70" t="n">
-        <v>24.67541766109792</v>
+        <v>3.916666666666667</v>
       </c>
       <c r="BM70" t="n">
-        <v>3.916666666666667</v>
+        <v>0.7999999999999989</v>
       </c>
       <c r="BN70" t="n">
-        <v>0.7999999999999989</v>
+        <v>3</v>
       </c>
       <c r="BO70" t="n">
-        <v>3</v>
+        <v>-1.9</v>
       </c>
       <c r="BP70" t="n">
-        <v>-1.9</v>
+        <v>1.789999999999999</v>
       </c>
       <c r="BQ70" t="n">
-        <v>1.789999999999999</v>
+        <v>16.73487101669205</v>
+      </c>
+      <c r="BR70" t="n">
+        <v>3.683333333333333</v>
+      </c>
+      <c r="BS70" t="n">
+        <v>5.194628341459548</v>
       </c>
     </row>
     <row r="71">
@@ -15322,25 +15746,31 @@
         <v>18.77536491677344</v>
       </c>
       <c r="BK71" t="n">
-        <v>16.85343465045614</v>
+        <v>20.19057007125899</v>
       </c>
       <c r="BL71" t="n">
-        <v>20.19057007125899</v>
+        <v>1.75</v>
       </c>
       <c r="BM71" t="n">
-        <v>1.75</v>
+        <v>0.6999999999999993</v>
       </c>
       <c r="BN71" t="n">
-        <v>0.6999999999999993</v>
+        <v>0.7100000000000009</v>
       </c>
       <c r="BO71" t="n">
-        <v>0.7100000000000009</v>
+        <v>-0.5</v>
       </c>
       <c r="BP71" t="n">
-        <v>-0.5</v>
+        <v>-1.609999999999999</v>
       </c>
       <c r="BQ71" t="n">
-        <v>-1.609999999999999</v>
+        <v>17.30430091185421</v>
+      </c>
+      <c r="BR71" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS71" t="n">
+        <v>1.471064004919235</v>
       </c>
     </row>
     <row r="72">
@@ -15531,25 +15961,31 @@
         <v>21.57331626120373</v>
       </c>
       <c r="BK72" t="n">
-        <v>16.10113808801217</v>
+        <v>23.34289786223287</v>
       </c>
       <c r="BL72" t="n">
-        <v>23.34289786223287</v>
+        <v>7.266666666666667</v>
       </c>
       <c r="BM72" t="n">
-        <v>7.266666666666667</v>
+        <v>0.7900000000000009</v>
       </c>
       <c r="BN72" t="n">
-        <v>0.7900000000000009</v>
+        <v>5.6</v>
       </c>
       <c r="BO72" t="n">
-        <v>5.6</v>
+        <v>-1.81</v>
       </c>
       <c r="BP72" t="n">
-        <v>-1.81</v>
+        <v>0.1000000000000014</v>
       </c>
       <c r="BQ72" t="n">
-        <v>0.1000000000000014</v>
+        <v>14.75894817073171</v>
+      </c>
+      <c r="BR72" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS72" t="n">
+        <v>6.814368090472023</v>
       </c>
     </row>
     <row r="73">
@@ -15740,25 +16176,31 @@
         <v>23.45815620998734</v>
       </c>
       <c r="BK73" t="n">
-        <v>16.71375000000007</v>
+        <v>27.90919239905</v>
       </c>
       <c r="BL73" t="n">
-        <v>27.90919239905</v>
+        <v>3.1</v>
       </c>
       <c r="BM73" t="n">
-        <v>3.1</v>
+        <v>1</v>
       </c>
       <c r="BN73" t="n">
-        <v>1</v>
+        <v>5.099999999999998</v>
       </c>
       <c r="BO73" t="n">
-        <v>5.099999999999998</v>
+        <v>-2.109999999999999</v>
       </c>
       <c r="BP73" t="n">
-        <v>-2.109999999999999</v>
+        <v>4</v>
       </c>
       <c r="BQ73" t="n">
-        <v>4</v>
+        <v>17.3675379939209</v>
+      </c>
+      <c r="BR73" t="n">
+        <v>0.7666666666666667</v>
+      </c>
+      <c r="BS73" t="n">
+        <v>6.090618216066442</v>
       </c>
     </row>
     <row r="74">
@@ -15949,25 +16391,31 @@
         <v>26.27039743589754</v>
       </c>
       <c r="BK74" t="n">
-        <v>19.34101823708203</v>
+        <v>29.00280952380963</v>
       </c>
       <c r="BL74" t="n">
-        <v>29.00280952380963</v>
+        <v>4.183333333333334</v>
       </c>
       <c r="BM74" t="n">
-        <v>4.183333333333334</v>
+        <v>2.1</v>
       </c>
       <c r="BN74" t="n">
-        <v>2.1</v>
+        <v>2.399999999999999</v>
       </c>
       <c r="BO74" t="n">
-        <v>2.399999999999999</v>
+        <v>-1.31</v>
       </c>
       <c r="BP74" t="n">
-        <v>-1.31</v>
+        <v>5.890000000000001</v>
       </c>
       <c r="BQ74" t="n">
-        <v>5.890000000000001</v>
+        <v>23.35389057750776</v>
+      </c>
+      <c r="BR74" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS74" t="n">
+        <v>2.916506858389788</v>
       </c>
     </row>
     <row r="75">
@@ -16158,25 +16606,31 @@
         <v>26.34227912932148</v>
       </c>
       <c r="BK75" t="n">
-        <v>23.74205167173269</v>
+        <v>26.82558194774358</v>
       </c>
       <c r="BL75" t="n">
-        <v>26.82558194774358</v>
+        <v>0</v>
       </c>
       <c r="BM75" t="n">
-        <v>0</v>
+        <v>1.41</v>
       </c>
       <c r="BN75" t="n">
-        <v>1.41</v>
+        <v>1.100000000000001</v>
       </c>
       <c r="BO75" t="n">
-        <v>1.100000000000001</v>
+        <v>6.699999999999999</v>
       </c>
       <c r="BP75" t="n">
-        <v>6.699999999999999</v>
+        <v>3.100000000000001</v>
       </c>
       <c r="BQ75" t="n">
-        <v>3.100000000000001</v>
+        <v>24.33557926829291</v>
+      </c>
+      <c r="BR75" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS75" t="n">
+        <v>2.006699861028562</v>
       </c>
     </row>
     <row r="76">
@@ -16367,25 +16821,31 @@
         <v>27.24962868117807</v>
       </c>
       <c r="BK76" t="n">
-        <v>24.0561128048782</v>
+        <v>27.90377672209043</v>
       </c>
       <c r="BL76" t="n">
-        <v>27.90377672209043</v>
+        <v>1.966666666666667</v>
       </c>
       <c r="BM76" t="n">
-        <v>1.966666666666667</v>
+        <v>0.5</v>
       </c>
       <c r="BN76" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="BO76" t="n">
-        <v>1</v>
+        <v>6.5</v>
       </c>
       <c r="BP76" t="n">
         <v>6.5</v>
       </c>
       <c r="BQ76" t="n">
-        <v>6.5</v>
+        <v>22.68773899848278</v>
+      </c>
+      <c r="BR76" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS76" t="n">
+        <v>4.561889682695288</v>
       </c>
     </row>
     <row r="77">
@@ -16576,25 +17036,31 @@
         <v>22.07667522464718</v>
       </c>
       <c r="BK77" t="n">
-        <v>20.14983282674796</v>
+        <v>22.35857142857147</v>
       </c>
       <c r="BL77" t="n">
-        <v>22.35857142857147</v>
+        <v>0</v>
       </c>
       <c r="BM77" t="n">
-        <v>0</v>
+        <v>0.2899999999999991</v>
       </c>
       <c r="BN77" t="n">
-        <v>0.2899999999999991</v>
+        <v>2.300000000000001</v>
       </c>
       <c r="BO77" t="n">
-        <v>2.300000000000001</v>
+        <v>2</v>
       </c>
       <c r="BP77" t="n">
-        <v>2</v>
+        <v>-0.1099999999999994</v>
       </c>
       <c r="BQ77" t="n">
-        <v>-0.1099999999999994</v>
+        <v>17.11983257229833</v>
+      </c>
+      <c r="BR77" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS77" t="n">
+        <v>4.956842652348847</v>
       </c>
     </row>
     <row r="78">
@@ -16785,25 +17251,31 @@
         <v>22.39875800256094</v>
       </c>
       <c r="BK78" t="n">
-        <v>16.72117199391174</v>
+        <v>25.67277909738726</v>
       </c>
       <c r="BL78" t="n">
-        <v>25.67277909738726</v>
+        <v>4.95</v>
       </c>
       <c r="BM78" t="n">
-        <v>4.95</v>
+        <v>2.910000000000002</v>
       </c>
       <c r="BN78" t="n">
-        <v>2.910000000000002</v>
+        <v>4.190000000000001</v>
       </c>
       <c r="BO78" t="n">
-        <v>4.190000000000001</v>
+        <v>-1.81</v>
       </c>
       <c r="BP78" t="n">
-        <v>-1.81</v>
+        <v>2</v>
       </c>
       <c r="BQ78" t="n">
-        <v>2</v>
+        <v>15.28905775075987</v>
+      </c>
+      <c r="BR78" t="n">
+        <v>9.733333333333333</v>
+      </c>
+      <c r="BS78" t="n">
+        <v>7.109700251801076</v>
       </c>
     </row>
     <row r="79">
@@ -16994,25 +17466,31 @@
         <v>23.07691516709525</v>
       </c>
       <c r="BK79" t="n">
-        <v>14.9346737481032</v>
+        <v>23.73749403341292</v>
       </c>
       <c r="BL79" t="n">
-        <v>23.73749403341292</v>
+        <v>7.666666666666667</v>
       </c>
       <c r="BM79" t="n">
-        <v>7.666666666666667</v>
+        <v>3.700000000000001</v>
       </c>
       <c r="BN79" t="n">
-        <v>3.700000000000001</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="BO79" t="n">
-        <v>5.100000000000001</v>
+        <v>-3.81</v>
       </c>
       <c r="BP79" t="n">
-        <v>-3.81</v>
+        <v>2.789999999999999</v>
       </c>
       <c r="BQ79" t="n">
-        <v>2.789999999999999</v>
+        <v>14.53301972685887</v>
+      </c>
+      <c r="BR79" t="n">
+        <v>1.166666666666667</v>
+      </c>
+      <c r="BS79" t="n">
+        <v>8.543895440236385</v>
       </c>
     </row>
     <row r="80">
@@ -17203,25 +17681,31 @@
         <v>24.09274007682466</v>
       </c>
       <c r="BK80" t="n">
-        <v>15.3335660091048</v>
+        <v>25.76904988123522</v>
       </c>
       <c r="BL80" t="n">
-        <v>25.76904988123522</v>
+        <v>3.883333333333333</v>
       </c>
       <c r="BM80" t="n">
-        <v>3.883333333333333</v>
+        <v>6.410000000000002</v>
       </c>
       <c r="BN80" t="n">
-        <v>6.410000000000002</v>
+        <v>3.399999999999999</v>
       </c>
       <c r="BO80" t="n">
-        <v>3.399999999999999</v>
+        <v>-4.31</v>
       </c>
       <c r="BP80" t="n">
-        <v>-4.31</v>
+        <v>2.289999999999999</v>
       </c>
       <c r="BQ80" t="n">
-        <v>2.289999999999999</v>
+        <v>16.60655538694993</v>
+      </c>
+      <c r="BR80" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="BS80" t="n">
+        <v>7.486184689874737</v>
       </c>
     </row>
     <row r="81">
@@ -17412,25 +17896,31 @@
         <v>23.70953905249692</v>
       </c>
       <c r="BK81" t="n">
-        <v>17.23561456752662</v>
+        <v>24.35862232779108</v>
       </c>
       <c r="BL81" t="n">
-        <v>24.35862232779108</v>
+        <v>4.35</v>
       </c>
       <c r="BM81" t="n">
-        <v>4.35</v>
+        <v>2.9</v>
       </c>
       <c r="BN81" t="n">
-        <v>2.9</v>
+        <v>1.600000000000001</v>
       </c>
       <c r="BO81" t="n">
-        <v>1.600000000000001</v>
+        <v>-1.9</v>
       </c>
       <c r="BP81" t="n">
-        <v>-1.9</v>
+        <v>3.789999999999999</v>
       </c>
       <c r="BQ81" t="n">
-        <v>3.789999999999999</v>
+        <v>19.27007587253434</v>
+      </c>
+      <c r="BR81" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS81" t="n">
+        <v>4.43946317996258</v>
       </c>
     </row>
     <row r="82">
@@ -17621,25 +18111,31 @@
         <v>25.17225352112685</v>
       </c>
       <c r="BK82" t="n">
-        <v>17.46779969650988</v>
+        <v>26.76966745843244</v>
       </c>
       <c r="BL82" t="n">
-        <v>26.76966745843244</v>
+        <v>3.233333333333333</v>
       </c>
       <c r="BM82" t="n">
-        <v>3.233333333333333</v>
+        <v>1.199999999999999</v>
       </c>
       <c r="BN82" t="n">
-        <v>1.199999999999999</v>
+        <v>5.189999999999998</v>
       </c>
       <c r="BO82" t="n">
-        <v>5.189999999999998</v>
+        <v>-2.31</v>
       </c>
       <c r="BP82" t="n">
-        <v>-2.31</v>
+        <v>3.699999999999999</v>
       </c>
       <c r="BQ82" t="n">
-        <v>3.699999999999999</v>
+        <v>13.99364741641346</v>
+      </c>
+      <c r="BR82" t="n">
+        <v>1.166666666666667</v>
+      </c>
+      <c r="BS82" t="n">
+        <v>11.17860610471339</v>
       </c>
     </row>
     <row r="83">
@@ -17830,25 +18326,31 @@
         <v>24.1118461538463</v>
       </c>
       <c r="BK83" t="n">
-        <v>14.64218844984804</v>
+        <v>26.92076009501201</v>
       </c>
       <c r="BL83" t="n">
-        <v>26.92076009501201</v>
+        <v>2.916666666666667</v>
       </c>
       <c r="BM83" t="n">
-        <v>2.916666666666667</v>
+        <v>2.5</v>
       </c>
       <c r="BN83" t="n">
-        <v>2.5</v>
+        <v>5.5</v>
       </c>
       <c r="BO83" t="n">
-        <v>5.5</v>
+        <v>-4.9</v>
       </c>
       <c r="BP83" t="n">
-        <v>-4.9</v>
+        <v>3.5</v>
       </c>
       <c r="BQ83" t="n">
-        <v>3.5</v>
+        <v>14.57723404255319</v>
+      </c>
+      <c r="BR83" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="BS83" t="n">
+        <v>9.534612111293104</v>
       </c>
     </row>
     <row r="84">
@@ -18039,234 +18541,31 @@
         <v>24.69285897435911</v>
       </c>
       <c r="BK84" t="n">
-        <v>15.36731003039518</v>
+        <v>27.5209738717341</v>
       </c>
       <c r="BL84" t="n">
-        <v>27.5209738717341</v>
+        <v>2.816666666666667</v>
       </c>
       <c r="BM84" t="n">
-        <v>2.816666666666667</v>
+        <v>4.1</v>
       </c>
       <c r="BN84" t="n">
-        <v>4.1</v>
+        <v>4.5</v>
       </c>
       <c r="BO84" t="n">
-        <v>4.5</v>
+        <v>-5</v>
       </c>
       <c r="BP84" t="n">
-        <v>-5</v>
+        <v>4</v>
       </c>
       <c r="BQ84" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n">
-        <v>20180526</v>
-      </c>
-      <c r="B85" t="n">
-        <v>22.60580264072276</v>
-      </c>
-      <c r="C85" t="n">
-        <v>71.63186240444645</v>
-      </c>
-      <c r="D85" t="n">
-        <v>16.18525865127521</v>
-      </c>
-      <c r="E85" t="n">
-        <v>7.844576452953729</v>
-      </c>
-      <c r="F85" t="n">
-        <v>0.897271088654428</v>
-      </c>
-      <c r="G85" t="n">
-        <v>2941.521534738077</v>
-      </c>
-      <c r="H85" t="n">
-        <v>0.01156146396462005</v>
-      </c>
-      <c r="I85" t="n">
-        <v>52.13912001631595</v>
-      </c>
-      <c r="J85" t="n">
-        <v>0.8536123101958799</v>
-      </c>
-      <c r="K85" t="n">
-        <v>1.172159071076051</v>
-      </c>
-      <c r="L85" t="n">
-        <v>1848.597108242295</v>
-      </c>
-      <c r="M85" t="n">
-        <v>13.52969951886967</v>
-      </c>
-      <c r="N85" t="n">
-        <v>21.37427597182338</v>
-      </c>
-      <c r="O85" t="n">
-        <v>6.667875681003868</v>
-      </c>
-      <c r="P85" t="n">
-        <v>23.321018780793</v>
-      </c>
-      <c r="Q85" t="n">
-        <v>1.860588942899734</v>
-      </c>
-      <c r="R85" t="n">
-        <v>7.479394693362138</v>
-      </c>
-      <c r="S85" t="n">
-        <v>0.3955394117954357</v>
-      </c>
-      <c r="T85" t="n">
-        <v>1143.245490285844</v>
-      </c>
-      <c r="U85" t="n">
-        <v>0.001388351995585361</v>
-      </c>
-      <c r="V85" t="n">
-        <v>9.293183409698694</v>
-      </c>
-      <c r="W85" t="n">
-        <v>0.02033818495684855</v>
-      </c>
-      <c r="X85" t="n">
-        <v>0.02802139075389157</v>
-      </c>
-      <c r="Y85" t="n">
-        <v>217.9772743086853</v>
-      </c>
-      <c r="Z85" t="n">
-        <v>1.458298792409421</v>
-      </c>
-      <c r="AA85" t="n">
-        <v>7.872520863396458</v>
-      </c>
-      <c r="AB85" t="n">
-        <v>12.8</v>
-      </c>
-      <c r="AC85" t="n">
-        <v>31.7</v>
-      </c>
-      <c r="AD85" t="n">
-        <v>12.6621538415837</v>
-      </c>
-      <c r="AE85" t="n">
-        <v>0.01147588697167556</v>
-      </c>
-      <c r="AF85" t="n">
-        <v>0.3502756118890946</v>
-      </c>
-      <c r="AG85" t="n">
-        <v>1478.324635686837</v>
-      </c>
-      <c r="AH85" t="n">
-        <v>0.00910622111552427</v>
-      </c>
-      <c r="AI85" t="n">
-        <v>35.86150310617688</v>
-      </c>
-      <c r="AJ85" t="n">
-        <v>0.8220894613444327</v>
-      </c>
-      <c r="AK85" t="n">
-        <v>1.128344690076635</v>
-      </c>
-      <c r="AL85" t="n">
-        <v>1462.063064694282</v>
-      </c>
-      <c r="AM85" t="n">
-        <v>10.48495601653669</v>
-      </c>
-      <c r="AN85" t="n">
-        <v>11.20202496016745</v>
-      </c>
-      <c r="AO85" t="n">
-        <v>32.59</v>
-      </c>
-      <c r="AP85" t="n">
-        <v>99.90000000000001</v>
-      </c>
-      <c r="AQ85" t="n">
-        <v>21.72295321531828</v>
-      </c>
-      <c r="AR85" t="n">
-        <v>22.64901093342938</v>
-      </c>
-      <c r="AS85" t="n">
-        <v>1.728728929414451</v>
-      </c>
-      <c r="AT85" t="n">
-        <v>4919.627655381318</v>
-      </c>
-      <c r="AU85" t="n">
-        <v>0.01637368284261791</v>
-      </c>
-      <c r="AV85" t="n">
-        <v>72.32119995534488</v>
-      </c>
-      <c r="AW85" t="n">
-        <v>0.8862540044674484</v>
-      </c>
-      <c r="AX85" t="n">
-        <v>1.216412625415019</v>
-      </c>
-      <c r="AY85" t="n">
-        <v>2598.972103740947</v>
-      </c>
-      <c r="AZ85" t="n">
-        <v>18.55861707311115</v>
-      </c>
-      <c r="BA85" t="n">
-        <v>34.86557207890262</v>
-      </c>
-      <c r="BB85" t="n">
-        <v>0.7833333333333333</v>
-      </c>
-      <c r="BC85" t="n">
-        <v>0.7833333333333333</v>
-      </c>
-      <c r="BD85" t="n">
-        <v>1.483333333333333</v>
-      </c>
-      <c r="BE85" t="n">
-        <v>4.916666666666667</v>
-      </c>
-      <c r="BF85" t="n">
-        <v>7.133333333333334</v>
-      </c>
-      <c r="BG85" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH85" t="n">
-        <v>4.366666666666666</v>
-      </c>
-      <c r="BI85" t="n">
-        <v>2.483333333333333</v>
-      </c>
-      <c r="BJ85" t="n">
-        <v>27.0558333333334</v>
-      </c>
-      <c r="BK85" t="n">
-        <v>17.33869499241286</v>
-      </c>
-      <c r="BL85" t="n">
-        <v>30.39420427553457</v>
-      </c>
-      <c r="BM85" t="n">
-        <v>2.583333333333333</v>
-      </c>
-      <c r="BN85" t="n">
-        <v>3.800000000000001</v>
-      </c>
-      <c r="BO85" t="n">
-        <v>5.190000000000001</v>
-      </c>
-      <c r="BP85" t="n">
-        <v>-3.199999999999999</v>
-      </c>
-      <c r="BQ85" t="n">
-        <v>6.590000000000003</v>
+        <v>16.43981790591802</v>
+      </c>
+      <c r="BR84" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="BS84" t="n">
+        <v>8.253041068441089</v>
       </c>
     </row>
   </sheetData>

</xml_diff>